<commit_message>
Aanpassing verwijzing GLD naar monitoringbuis, en omgekeerd
Aanpassing brondatamodel en mappings: GLD- en GMW-objecten verwijzen nu naar elkaars Bron-ID, meerdere GLD-objecten kunnen ook verwijzen naar dezelfde monitoringbuis (d.GMW.Tube.GLDID kan evt een lijst zijn, verwijzing vanuit d.GMW.Tube naar GLD mag uitgefaseerd worden).
</commit_message>
<xml_diff>
--- a/BROMappings/Mapping en definitie BRO GLD.xlsx
+++ b/BROMappings/Mapping en definitie BRO GLD.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/trunk/BronDatamodel/BROMappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{BE372826-5466-43B2-95C7-E0F7EC2978EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DC57D00-8273-4EFA-9B96-C7E8B94F4478}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{BE372826-5466-43B2-95C7-E0F7EC2978EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C026CC9D-0A24-4DF5-83E8-A63DDCA499B2}"/>
   <bookViews>
-    <workbookView xWindow="19548" yWindow="2100" windowWidth="21600" windowHeight="11328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-5490" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="260">
   <si>
     <t>Opmerking</t>
   </si>
@@ -802,6 +802,12 @@
   </si>
   <si>
     <t xml:space="preserve">Opname van ID bij 1 : n relatie vereenvoudigt tabeloperaties (bijv. innerjoin) </t>
+  </si>
+  <si>
+    <t>T.b.v. relatie met putten die nog niet geregistreerd zijn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMWID </t>
   </si>
 </sst>
 </file>
@@ -1232,39 +1238,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T235"/>
+  <dimension ref="A1:T236"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3636" ySplit="564" topLeftCell="O1" activePane="bottomRight"/>
+      <pane xSplit="3630" ySplit="570" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
-      <selection pane="bottomRight" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="60.5703125" style="8" customWidth="1"/>
-    <col min="15" max="17" width="25.28515625" customWidth="1"/>
-    <col min="18" max="18" width="26.28515625" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="77.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.5546875" style="8" customWidth="1"/>
+    <col min="15" max="17" width="25.33203125" customWidth="1"/>
+    <col min="18" max="18" width="26.33203125" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="77.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1326,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>179</v>
       </c>
@@ -1375,7 +1381,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -1406,13 +1412,13 @@
       </c>
       <c r="N3"/>
       <c r="O3" t="s">
-        <v>223</v>
+        <v>173</v>
       </c>
       <c r="P3" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="Q3" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="R3" s="18" t="s">
         <v>175</v>
@@ -1421,98 +1427,107 @@
         <v>220</v>
       </c>
       <c r="T3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L4" t="s">
+        <v>196</v>
+      </c>
+      <c r="M4" t="s">
+        <v>196</v>
+      </c>
+      <c r="N4"/>
+      <c r="O4" t="s">
+        <v>223</v>
+      </c>
+      <c r="P4" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>256</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="S4" t="s">
+        <v>220</v>
+      </c>
+      <c r="T4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="N4" s="16"/>
-      <c r="O4" s="1" t="s">
+    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="N5" s="16"/>
+      <c r="O5" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="R4" s="17" t="s">
+      <c r="R5" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B5"/>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="N5"/>
-      <c r="O5" t="s">
-        <v>217</v>
-      </c>
-      <c r="P5" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>174</v>
-      </c>
-      <c r="R5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>185</v>
       </c>
@@ -1524,13 +1539,13 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1538,23 +1553,21 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="N6" t="s">
-        <v>49</v>
-      </c>
+      <c r="N6"/>
       <c r="O6" t="s">
         <v>217</v>
       </c>
       <c r="P6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Q6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="R6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>185</v>
       </c>
@@ -1566,13 +1579,13 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1581,255 +1594,255 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O7" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="P7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Q7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="R7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>185</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" t="s">
+        <v>179</v>
+      </c>
+      <c r="P8" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>179</v>
+      </c>
+      <c r="R8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9"/>
+      <c r="C9" t="s">
         <v>244</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>245</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>243</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>38</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>32</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
         <v>220</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N9" t="s">
         <v>51</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O9" t="s">
         <v>217</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P9" t="s">
         <v>246</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q9" t="s">
         <v>246</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="R9" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="1">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1">
-        <v>1</v>
-      </c>
-      <c r="N9" s="1" t="s">
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>186</v>
       </c>
-      <c r="B10"/>
-      <c r="C10" t="s">
+      <c r="B11"/>
+      <c r="C11" t="s">
         <v>69</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>70</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>57</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>94</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
         <v>82</v>
-      </c>
-      <c r="O10" t="s">
-        <v>217</v>
-      </c>
-      <c r="P10" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>191</v>
-      </c>
-      <c r="R10" t="s">
-        <v>183</v>
-      </c>
-      <c r="T10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="O11" t="s">
         <v>217</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>191</v>
+      </c>
+      <c r="R11" t="s">
+        <v>183</v>
+      </c>
+      <c r="T11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O12" t="s">
+        <v>217</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R12" t="s">
         <v>184</v>
       </c>
-      <c r="S11"/>
-      <c r="T11" s="1" t="s">
+      <c r="S12"/>
+      <c r="T12" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>186</v>
-      </c>
-      <c r="B12"/>
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
-        <v>83</v>
-      </c>
-      <c r="O12" t="s">
-        <v>189</v>
-      </c>
-      <c r="P12" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>189</v>
-      </c>
-      <c r="R12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>186</v>
       </c>
@@ -1841,22 +1854,22 @@
         <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O13" t="s">
         <v>189</v>
@@ -1868,13 +1881,10 @@
         <v>189</v>
       </c>
       <c r="R13" t="s">
-        <v>183</v>
-      </c>
-      <c r="T13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>186</v>
       </c>
@@ -1886,10 +1896,10 @@
         <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" t="s">
         <v>94</v>
@@ -1901,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O14" t="s">
         <v>189</v>
@@ -1915,8 +1925,11 @@
       <c r="R14" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>186</v>
       </c>
@@ -1928,22 +1941,22 @@
         <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O15" t="s">
         <v>189</v>
@@ -1955,10 +1968,10 @@
         <v>189</v>
       </c>
       <c r="R15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>186</v>
       </c>
@@ -1970,22 +1983,22 @@
         <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O16" t="s">
         <v>189</v>
@@ -1997,10 +2010,10 @@
         <v>189</v>
       </c>
       <c r="R16" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>186</v>
       </c>
@@ -2012,22 +2025,22 @@
         <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O17" t="s">
         <v>189</v>
@@ -2039,10 +2052,10 @@
         <v>189</v>
       </c>
       <c r="R17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>186</v>
       </c>
@@ -2054,22 +2067,22 @@
         <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O18" t="s">
         <v>189</v>
@@ -2081,10 +2094,10 @@
         <v>189</v>
       </c>
       <c r="R18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>186</v>
       </c>
@@ -2096,22 +2109,22 @@
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H19" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O19" t="s">
         <v>189</v>
@@ -2123,10 +2136,10 @@
         <v>189</v>
       </c>
       <c r="R19" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -2138,22 +2151,22 @@
         <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O20" t="s">
         <v>189</v>
@@ -2165,10 +2178,10 @@
         <v>189</v>
       </c>
       <c r="R20" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>186</v>
       </c>
@@ -2180,256 +2193,253 @@
         <v>47</v>
       </c>
       <c r="E21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" t="s">
+        <v>94</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>91</v>
+      </c>
+      <c r="O21" t="s">
+        <v>189</v>
+      </c>
+      <c r="P21" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>189</v>
+      </c>
+      <c r="R21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
         <v>80</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>67</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>34</v>
       </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
         <v>92</v>
       </c>
-      <c r="O21" t="s">
-        <v>189</v>
-      </c>
-      <c r="P21" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>189</v>
-      </c>
-      <c r="R21" t="s">
+      <c r="O22" t="s">
+        <v>189</v>
+      </c>
+      <c r="P22" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>189</v>
+      </c>
+      <c r="R22" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J23" s="1">
         <v>0</v>
       </c>
-      <c r="K22" s="1">
-        <v>1</v>
-      </c>
-      <c r="N22" s="1" t="s">
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O22" t="s">
-        <v>189</v>
-      </c>
-      <c r="P22" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>189</v>
-      </c>
-      <c r="R22" s="1" t="s">
+      <c r="O23" t="s">
+        <v>189</v>
+      </c>
+      <c r="P23" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>189</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="S22"/>
-    </row>
-    <row r="23" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="S23"/>
+    </row>
+    <row r="24" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="9" t="s">
+      <c r="F24" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="9">
-        <v>1</v>
-      </c>
-      <c r="K23" s="9">
-        <v>1</v>
-      </c>
-      <c r="N23" s="9" t="s">
+      <c r="J24" s="9">
+        <v>1</v>
+      </c>
+      <c r="K24" s="9">
+        <v>1</v>
+      </c>
+      <c r="N24" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="O23" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="P23" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q23" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="R23" s="9" t="s">
+      <c r="O24" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="R24" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="S23"/>
-    </row>
-    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="S24"/>
+    </row>
+    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>186</v>
       </c>
-      <c r="B24"/>
-      <c r="C24" t="s">
+      <c r="B25"/>
+      <c r="C25" t="s">
         <v>97</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>31</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>27</v>
       </c>
-      <c r="F24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="F25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
         <v>53</v>
       </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="N24" t="s">
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="N25" t="s">
         <v>98</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O25" t="s">
         <v>173</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P25" t="s">
         <v>247</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q25" t="s">
         <v>247</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R25" t="s">
         <v>216</v>
       </c>
-      <c r="T24" t="s">
+      <c r="T25" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="1">
-        <v>1</v>
-      </c>
-      <c r="K25" s="1">
-        <v>1</v>
-      </c>
-      <c r="N25" s="1" t="s">
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="S25"/>
-      <c r="T25" s="1" t="s">
+      <c r="S26"/>
+      <c r="T26" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>186</v>
-      </c>
-      <c r="B26"/>
-      <c r="C26" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" t="s">
-        <v>47</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="M26" t="s">
-        <v>188</v>
-      </c>
-      <c r="N26" t="s">
-        <v>54</v>
-      </c>
-      <c r="O26" t="s">
-        <v>189</v>
-      </c>
-      <c r="P26" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>189</v>
-      </c>
-      <c r="R26" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>186</v>
       </c>
@@ -2441,16 +2451,16 @@
         <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -2459,109 +2469,112 @@
         <v>188</v>
       </c>
       <c r="N27" t="s">
+        <v>54</v>
+      </c>
+      <c r="O27" t="s">
+        <v>189</v>
+      </c>
+      <c r="P27" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>189</v>
+      </c>
+      <c r="R27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>186</v>
+      </c>
+      <c r="B28"/>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>188</v>
+      </c>
+      <c r="N28" t="s">
         <v>55</v>
       </c>
-      <c r="O27" t="s">
-        <v>189</v>
-      </c>
-      <c r="P27" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>189</v>
-      </c>
-      <c r="R27" t="s">
+      <c r="O28" t="s">
+        <v>189</v>
+      </c>
+      <c r="P28" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>189</v>
+      </c>
+      <c r="R28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J29" s="1">
         <v>0</v>
       </c>
-      <c r="K28" s="1">
-        <v>1</v>
-      </c>
-      <c r="M28" s="1" t="s">
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="R28" s="1" t="s">
+      <c r="O29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R29" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="S28"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>186</v>
-      </c>
-      <c r="B29"/>
-      <c r="C29" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" t="s">
-        <v>100</v>
-      </c>
-      <c r="H29" t="s">
-        <v>33</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29" t="s">
-        <v>172</v>
-      </c>
-      <c r="N29" t="s">
-        <v>108</v>
-      </c>
-      <c r="O29" t="s">
-        <v>223</v>
-      </c>
-      <c r="P29" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>211</v>
-      </c>
-      <c r="R29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S29"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>186</v>
       </c>
@@ -2573,13 +2586,13 @@
         <v>106</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H30" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -2588,108 +2601,105 @@
         <v>172</v>
       </c>
       <c r="N30" t="s">
+        <v>108</v>
+      </c>
+      <c r="O30" t="s">
+        <v>223</v>
+      </c>
+      <c r="P30" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>211</v>
+      </c>
+      <c r="R30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31"/>
+      <c r="C31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" t="s">
+        <v>101</v>
+      </c>
+      <c r="H31" t="s">
+        <v>111</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31" t="s">
+        <v>172</v>
+      </c>
+      <c r="N31" t="s">
         <v>109</v>
       </c>
-      <c r="O30" t="s">
-        <v>189</v>
-      </c>
-      <c r="P30" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>189</v>
-      </c>
-      <c r="R30" t="s">
+      <c r="O31" t="s">
+        <v>189</v>
+      </c>
+      <c r="P31" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>189</v>
+      </c>
+      <c r="R31" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J32" s="1">
         <v>0</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="N32" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O31" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="R31" s="1" t="s">
+      <c r="O32" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R32" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>186</v>
-      </c>
-      <c r="B32"/>
-      <c r="C32" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" t="s">
-        <v>113</v>
-      </c>
-      <c r="H32" t="s">
-        <v>48</v>
-      </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-      <c r="K32" t="s">
-        <v>172</v>
-      </c>
-      <c r="N32" t="s">
-        <v>121</v>
-      </c>
-      <c r="O32" t="s">
-        <v>189</v>
-      </c>
-      <c r="P32" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>189</v>
-      </c>
-      <c r="R32" t="s">
-        <v>183</v>
-      </c>
-      <c r="T32" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -2701,13 +2711,13 @@
         <v>112</v>
       </c>
       <c r="E33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H33" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -2716,191 +2726,191 @@
         <v>172</v>
       </c>
       <c r="N33" t="s">
+        <v>121</v>
+      </c>
+      <c r="O33" t="s">
+        <v>189</v>
+      </c>
+      <c r="P33" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>189</v>
+      </c>
+      <c r="R33" t="s">
+        <v>183</v>
+      </c>
+      <c r="T33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34"/>
+      <c r="C34" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" t="s">
+        <v>114</v>
+      </c>
+      <c r="H34" t="s">
+        <v>34</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>172</v>
+      </c>
+      <c r="N34" t="s">
         <v>122</v>
       </c>
-      <c r="O33" t="s">
-        <v>189</v>
-      </c>
-      <c r="P33" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>189</v>
-      </c>
-      <c r="R33" t="s">
+      <c r="O34" t="s">
+        <v>189</v>
+      </c>
+      <c r="P34" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>189</v>
+      </c>
+      <c r="R34" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J35" s="1">
         <v>0</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="P34" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="Q35" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="R34" s="1" t="s">
+      <c r="R35" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>186</v>
       </c>
-      <c r="B35"/>
-      <c r="C35" t="s">
+      <c r="B36"/>
+      <c r="C36" t="s">
         <v>129</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>120</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>248</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>124</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H36" t="s">
         <v>32</v>
       </c>
-      <c r="J35">
+      <c r="J36">
         <v>0</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K36" t="s">
         <v>172</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N36" t="s">
         <v>127</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O36" t="s">
         <v>223</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P36" t="s">
         <v>194</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="Q36" t="s">
         <v>194</v>
       </c>
-      <c r="R35" t="s">
+      <c r="R36" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J37" s="1">
         <v>0</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="O36" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="R36" s="1" t="s">
+      <c r="O37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R37" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>186</v>
-      </c>
-      <c r="B37"/>
-      <c r="C37" t="s">
-        <v>148</v>
-      </c>
-      <c r="D37" t="s">
-        <v>149</v>
-      </c>
-      <c r="E37" t="s">
-        <v>136</v>
-      </c>
-      <c r="F37" t="s">
-        <v>130</v>
-      </c>
-      <c r="H37" t="s">
-        <v>33</v>
-      </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="N37" t="s">
-        <v>142</v>
-      </c>
-      <c r="O37" t="s">
-        <v>223</v>
-      </c>
-      <c r="P37" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>210</v>
-      </c>
-      <c r="R37" t="s">
-        <v>184</v>
-      </c>
-      <c r="T37" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>186</v>
       </c>
@@ -2912,13 +2922,13 @@
         <v>149</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -2927,25 +2937,25 @@
         <v>1</v>
       </c>
       <c r="N38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O38" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="P38" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="Q38" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="R38" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="T38" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -2957,10 +2967,10 @@
         <v>149</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H39" t="s">
         <v>34</v>
@@ -2972,7 +2982,7 @@
         <v>1</v>
       </c>
       <c r="N39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O39" t="s">
         <v>189</v>
@@ -2990,7 +3000,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>186</v>
       </c>
@@ -3002,10 +3012,10 @@
         <v>149</v>
       </c>
       <c r="E40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H40" t="s">
         <v>34</v>
@@ -3017,7 +3027,7 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O40" t="s">
         <v>189</v>
@@ -3035,7 +3045,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -3047,10 +3057,10 @@
         <v>149</v>
       </c>
       <c r="E41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H41" t="s">
         <v>34</v>
@@ -3062,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="N41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O41" t="s">
         <v>189</v>
@@ -3076,180 +3086,180 @@
       <c r="R41" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="T41" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>186</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42"/>
+      <c r="C42" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>149</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42" t="s">
+        <v>134</v>
+      </c>
+      <c r="H42" t="s">
+        <v>34</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="N42" t="s">
+        <v>146</v>
+      </c>
+      <c r="O42" t="s">
+        <v>189</v>
+      </c>
+      <c r="P42" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>189</v>
+      </c>
+      <c r="R42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J42" s="1">
-        <v>1</v>
-      </c>
-      <c r="K42" s="1">
-        <v>1</v>
-      </c>
-      <c r="N42" s="1" t="s">
+      <c r="J43" s="1">
+        <v>1</v>
+      </c>
+      <c r="K43" s="1">
+        <v>1</v>
+      </c>
+      <c r="N43" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="O42" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="R42" s="1" t="s">
+      <c r="O43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R43" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="T42" s="1" t="s">
+      <c r="T43" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>186</v>
       </c>
-      <c r="B43"/>
-      <c r="C43" t="s">
+      <c r="B44"/>
+      <c r="C44" t="s">
         <v>157</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>156</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>152</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F44" t="s">
         <v>150</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H44" t="s">
         <v>94</v>
       </c>
-      <c r="J43">
-        <v>1</v>
-      </c>
-      <c r="K43" t="s">
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44" t="s">
         <v>172</v>
       </c>
-      <c r="N43" t="s">
+      <c r="N44" t="s">
         <v>154</v>
       </c>
-      <c r="O43" t="s">
-        <v>189</v>
-      </c>
-      <c r="P43" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>189</v>
-      </c>
-      <c r="R43" t="s">
+      <c r="O44" t="s">
+        <v>189</v>
+      </c>
+      <c r="P44" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>189</v>
+      </c>
+      <c r="R44" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J44" s="1">
-        <v>1</v>
-      </c>
-      <c r="K44" s="1" t="s">
+      <c r="J45" s="1">
+        <v>1</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="O44" t="s">
-        <v>189</v>
-      </c>
-      <c r="P44" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>189</v>
-      </c>
-      <c r="R44" s="1" t="s">
+      <c r="O45" t="s">
+        <v>189</v>
+      </c>
+      <c r="P45" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>189</v>
+      </c>
+      <c r="R45" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>186</v>
-      </c>
-      <c r="B45"/>
-      <c r="C45" t="s">
-        <v>166</v>
-      </c>
-      <c r="D45" t="s">
-        <v>167</v>
-      </c>
-      <c r="E45" t="s">
-        <v>162</v>
-      </c>
-      <c r="F45" t="s">
-        <v>158</v>
-      </c>
-      <c r="H45" t="s">
-        <v>34</v>
-      </c>
-      <c r="J45">
-        <v>1</v>
-      </c>
-      <c r="K45" t="s">
-        <v>172</v>
-      </c>
-      <c r="N45" t="s">
-        <v>168</v>
-      </c>
-      <c r="O45" t="s">
-        <v>189</v>
-      </c>
-      <c r="P45" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>189</v>
-      </c>
-      <c r="R45" t="s">
-        <v>182</v>
-      </c>
-      <c r="T45" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>186</v>
       </c>
@@ -3261,22 +3271,22 @@
         <v>167</v>
       </c>
       <c r="E46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H46" t="s">
         <v>34</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" t="s">
         <v>172</v>
       </c>
       <c r="N46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O46" t="s">
         <v>189</v>
@@ -3290,8 +3300,11 @@
       <c r="R46" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T46" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>186</v>
       </c>
@@ -3303,13 +3316,13 @@
         <v>167</v>
       </c>
       <c r="E47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -3318,156 +3331,147 @@
         <v>172</v>
       </c>
       <c r="N47" t="s">
+        <v>169</v>
+      </c>
+      <c r="O47" t="s">
+        <v>189</v>
+      </c>
+      <c r="P47" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>189</v>
+      </c>
+      <c r="R47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48"/>
+      <c r="C48" t="s">
+        <v>166</v>
+      </c>
+      <c r="D48" t="s">
+        <v>167</v>
+      </c>
+      <c r="E48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F48" t="s">
+        <v>160</v>
+      </c>
+      <c r="H48" t="s">
+        <v>35</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48" t="s">
+        <v>172</v>
+      </c>
+      <c r="N48" t="s">
         <v>170</v>
       </c>
-      <c r="O47" t="s">
-        <v>189</v>
-      </c>
-      <c r="P47" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>189</v>
-      </c>
-      <c r="R47" t="s">
+      <c r="O48" t="s">
+        <v>189</v>
+      </c>
+      <c r="P48" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>189</v>
+      </c>
+      <c r="R48" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+    <row r="49" spans="1:20" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H49" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J48" s="4">
-        <v>1</v>
-      </c>
-      <c r="K48" s="4" t="s">
+      <c r="J49" s="4">
+        <v>1</v>
+      </c>
+      <c r="K49" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="N48" s="4" t="s">
+      <c r="N49" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="O48" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="P48" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q48" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="R48" s="4" t="s">
+      <c r="O49" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="R49" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
+    <row r="50" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C50" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D50" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E50" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F50" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="J49" s="13">
+      <c r="J50" s="13">
         <v>0</v>
       </c>
-      <c r="K49" s="13" t="s">
+      <c r="K50" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="M49" s="12" t="s">
+      <c r="M50" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="N49" s="14"/>
-      <c r="O49" s="12" t="s">
+      <c r="N50" s="14"/>
+      <c r="O50" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="P49" s="12" t="s">
+      <c r="P50" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="Q49" s="12" t="s">
+      <c r="Q50" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="R49" s="15" t="s">
+      <c r="R50" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="T49" s="12" t="s">
+      <c r="T50" s="12" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>179</v>
-      </c>
-      <c r="B50"/>
-      <c r="C50" t="s">
-        <v>179</v>
-      </c>
-      <c r="D50" t="s">
-        <v>179</v>
-      </c>
-      <c r="E50" t="s">
-        <v>179</v>
-      </c>
-      <c r="F50" t="s">
-        <v>179</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="L50" t="s">
-        <v>196</v>
-      </c>
-      <c r="M50" t="s">
-        <v>196</v>
-      </c>
-      <c r="O50" t="s">
-        <v>218</v>
-      </c>
-      <c r="P50" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>254</v>
-      </c>
-      <c r="R50" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>179</v>
       </c>
@@ -3509,19 +3513,16 @@
         <v>218</v>
       </c>
       <c r="P51" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
       <c r="Q51" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
       <c r="R51" t="s">
-        <v>184</v>
-      </c>
-      <c r="T51" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>179</v>
       </c>
@@ -3563,16 +3564,19 @@
         <v>218</v>
       </c>
       <c r="P52" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="Q52" t="s">
-        <v>219</v>
-      </c>
-      <c r="R52" s="10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="R52" t="s">
+        <v>184</v>
+      </c>
+      <c r="T52" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>179</v>
       </c>
@@ -3589,42 +3593,41 @@
       <c r="F53" t="s">
         <v>179</v>
       </c>
-      <c r="G53" t="s">
-        <v>179</v>
-      </c>
-      <c r="H53" t="s">
-        <v>179</v>
-      </c>
-      <c r="I53" t="s">
-        <v>179</v>
-      </c>
-      <c r="J53" t="s">
-        <v>179</v>
-      </c>
-      <c r="K53" t="s">
-        <v>179</v>
+      <c r="G53" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="L53" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="M53" t="s">
-        <v>179</v>
-      </c>
-      <c r="N53"/>
+        <v>196</v>
+      </c>
       <c r="O53" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="P53" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="Q53" t="s">
-        <v>198</v>
-      </c>
-      <c r="R53" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="R53" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>179</v>
       </c>
@@ -3641,41 +3644,42 @@
       <c r="F54" t="s">
         <v>179</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>196</v>
+      <c r="G54" t="s">
+        <v>179</v>
+      </c>
+      <c r="H54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I54" t="s">
+        <v>179</v>
+      </c>
+      <c r="J54" t="s">
+        <v>179</v>
+      </c>
+      <c r="K54" t="s">
+        <v>179</v>
       </c>
       <c r="L54" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="M54" t="s">
-        <v>196</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="N54"/>
       <c r="O54" t="s">
         <v>223</v>
       </c>
       <c r="P54" t="s">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="Q54" t="s">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="R54" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -3717,16 +3721,16 @@
         <v>223</v>
       </c>
       <c r="P55" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Q55" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="R55" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>179</v>
       </c>
@@ -3743,45 +3747,41 @@
       <c r="F56" t="s">
         <v>179</v>
       </c>
-      <c r="G56" t="s">
-        <v>179</v>
-      </c>
-      <c r="H56" t="s">
-        <v>179</v>
-      </c>
-      <c r="I56" t="s">
-        <v>179</v>
-      </c>
-      <c r="J56" t="s">
-        <v>179</v>
-      </c>
-      <c r="K56" t="s">
-        <v>179</v>
+      <c r="G56" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="L56" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="M56" t="s">
-        <v>179</v>
-      </c>
-      <c r="N56"/>
+        <v>196</v>
+      </c>
       <c r="O56" t="s">
         <v>223</v>
       </c>
       <c r="P56" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="Q56" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="R56" t="s">
-        <v>178</v>
-      </c>
-      <c r="T56" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>179</v>
       </c>
@@ -3824,16 +3824,19 @@
         <v>223</v>
       </c>
       <c r="P57" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="Q57" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="R57" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="T57" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>179</v>
       </c>
@@ -3876,16 +3879,16 @@
         <v>223</v>
       </c>
       <c r="P58" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q58" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="R58" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -3928,16 +3931,16 @@
         <v>223</v>
       </c>
       <c r="P59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R59" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>179</v>
       </c>
@@ -3980,16 +3983,16 @@
         <v>223</v>
       </c>
       <c r="P60" t="s">
-        <v>206</v>
+        <v>234</v>
       </c>
       <c r="Q60" t="s">
-        <v>206</v>
+        <v>234</v>
       </c>
       <c r="R60" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>179</v>
       </c>
@@ -4032,16 +4035,16 @@
         <v>223</v>
       </c>
       <c r="P61" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Q61" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R61" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -4084,19 +4087,16 @@
         <v>223</v>
       </c>
       <c r="P62" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="Q62" t="s">
-        <v>222</v>
-      </c>
-      <c r="R62" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="T62" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="R62" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>179</v>
       </c>
@@ -4139,19 +4139,19 @@
         <v>223</v>
       </c>
       <c r="P63" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="Q63" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="R63" s="10" t="s">
         <v>200</v>
       </c>
       <c r="T63" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>179</v>
       </c>
@@ -4194,16 +4194,19 @@
         <v>223</v>
       </c>
       <c r="P64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="Q64" t="s">
-        <v>201</v>
-      </c>
-      <c r="R64" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="R64" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="T64" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>179</v>
       </c>
@@ -4246,16 +4249,16 @@
         <v>223</v>
       </c>
       <c r="P65" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="Q65" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="R65" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>179</v>
       </c>
@@ -4298,1200 +4301,1252 @@
         <v>223</v>
       </c>
       <c r="P66" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>204</v>
+      </c>
+      <c r="R66" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>179</v>
+      </c>
+      <c r="B67"/>
+      <c r="C67" t="s">
+        <v>179</v>
+      </c>
+      <c r="D67" t="s">
+        <v>179</v>
+      </c>
+      <c r="E67" t="s">
+        <v>179</v>
+      </c>
+      <c r="F67" t="s">
+        <v>179</v>
+      </c>
+      <c r="G67" t="s">
+        <v>179</v>
+      </c>
+      <c r="H67" t="s">
+        <v>179</v>
+      </c>
+      <c r="I67" t="s">
+        <v>179</v>
+      </c>
+      <c r="J67" t="s">
+        <v>179</v>
+      </c>
+      <c r="K67" t="s">
+        <v>179</v>
+      </c>
+      <c r="L67" t="s">
+        <v>179</v>
+      </c>
+      <c r="M67" t="s">
+        <v>179</v>
+      </c>
+      <c r="N67"/>
+      <c r="O67" t="s">
+        <v>223</v>
+      </c>
+      <c r="P67" t="s">
         <v>203</v>
       </c>
-      <c r="Q66" t="s">
+      <c r="Q67" t="s">
         <v>203</v>
       </c>
-      <c r="R66" t="s">
+      <c r="R67" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="J67"/>
-      <c r="K67"/>
-      <c r="N67"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68"/>
       <c r="J68"/>
       <c r="K68"/>
       <c r="N68"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69"/>
       <c r="J69"/>
       <c r="K69"/>
       <c r="N69"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70"/>
       <c r="J70"/>
       <c r="K70"/>
       <c r="N70"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71"/>
       <c r="J71"/>
       <c r="K71"/>
       <c r="N71"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72"/>
       <c r="J72"/>
       <c r="K72"/>
       <c r="N72"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73"/>
       <c r="J73"/>
       <c r="K73"/>
       <c r="N73"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74"/>
       <c r="J74"/>
       <c r="K74"/>
       <c r="N74"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75"/>
       <c r="J75"/>
       <c r="K75"/>
       <c r="N75"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="B76"/>
       <c r="J76"/>
       <c r="K76"/>
       <c r="N76"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="B77"/>
       <c r="J77"/>
       <c r="K77"/>
       <c r="N77"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="B78"/>
       <c r="J78"/>
       <c r="K78"/>
       <c r="N78"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="B79"/>
       <c r="J79"/>
       <c r="K79"/>
       <c r="N79"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="J80"/>
       <c r="K80"/>
       <c r="N80"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81"/>
       <c r="B81"/>
       <c r="J81"/>
       <c r="K81"/>
       <c r="N81"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82"/>
       <c r="B82"/>
       <c r="J82"/>
       <c r="K82"/>
       <c r="N82"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83"/>
       <c r="B83"/>
       <c r="J83"/>
       <c r="K83"/>
       <c r="N83"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="B84"/>
       <c r="J84"/>
       <c r="K84"/>
       <c r="N84"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85"/>
       <c r="J85"/>
       <c r="K85"/>
       <c r="N85"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="B86"/>
       <c r="J86"/>
       <c r="K86"/>
       <c r="N86"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="B87"/>
       <c r="J87"/>
       <c r="K87"/>
       <c r="N87"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88"/>
       <c r="J88"/>
       <c r="K88"/>
       <c r="N88"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89"/>
       <c r="J89"/>
       <c r="K89"/>
       <c r="N89"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90"/>
       <c r="J90"/>
       <c r="K90"/>
       <c r="N90"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91"/>
       <c r="J91"/>
       <c r="K91"/>
       <c r="N91"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="B92"/>
       <c r="J92"/>
       <c r="K92"/>
       <c r="N92"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="B93"/>
       <c r="J93"/>
       <c r="K93"/>
       <c r="N93"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94"/>
       <c r="B94"/>
       <c r="J94"/>
       <c r="K94"/>
       <c r="N94"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95"/>
       <c r="B95"/>
       <c r="J95"/>
       <c r="K95"/>
       <c r="N95"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96"/>
       <c r="B96"/>
       <c r="J96"/>
       <c r="K96"/>
       <c r="N96"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97"/>
       <c r="B97"/>
       <c r="J97"/>
       <c r="K97"/>
       <c r="N97"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98"/>
       <c r="B98"/>
       <c r="J98"/>
       <c r="K98"/>
       <c r="N98"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99"/>
       <c r="B99"/>
       <c r="J99"/>
       <c r="K99"/>
       <c r="N99"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100"/>
       <c r="B100"/>
       <c r="J100"/>
       <c r="K100"/>
       <c r="N100"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101"/>
       <c r="B101"/>
       <c r="J101"/>
       <c r="K101"/>
       <c r="N101"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102"/>
       <c r="B102"/>
       <c r="J102"/>
       <c r="K102"/>
       <c r="N102"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103"/>
       <c r="B103"/>
       <c r="J103"/>
       <c r="K103"/>
       <c r="N103"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104"/>
       <c r="B104"/>
       <c r="J104"/>
       <c r="K104"/>
       <c r="N104"/>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105"/>
       <c r="B105"/>
       <c r="J105"/>
       <c r="K105"/>
       <c r="N105"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106"/>
       <c r="B106"/>
       <c r="J106"/>
       <c r="K106"/>
       <c r="N106"/>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107"/>
       <c r="B107"/>
       <c r="J107"/>
       <c r="K107"/>
       <c r="N107"/>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108"/>
       <c r="B108"/>
       <c r="J108"/>
       <c r="K108"/>
       <c r="N108"/>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109"/>
       <c r="B109"/>
       <c r="J109"/>
       <c r="K109"/>
       <c r="N109"/>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110"/>
       <c r="B110"/>
       <c r="J110"/>
       <c r="K110"/>
       <c r="N110"/>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111"/>
       <c r="B111"/>
       <c r="J111"/>
       <c r="K111"/>
       <c r="N111"/>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112"/>
       <c r="B112"/>
       <c r="J112"/>
       <c r="K112"/>
       <c r="N112"/>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113"/>
       <c r="B113"/>
       <c r="J113"/>
       <c r="K113"/>
       <c r="N113"/>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114"/>
       <c r="B114"/>
       <c r="J114"/>
       <c r="K114"/>
       <c r="N114"/>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115"/>
       <c r="B115"/>
       <c r="J115"/>
       <c r="K115"/>
       <c r="N115"/>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116"/>
       <c r="B116"/>
       <c r="J116"/>
       <c r="K116"/>
       <c r="N116"/>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117"/>
       <c r="B117"/>
       <c r="J117"/>
       <c r="K117"/>
       <c r="N117"/>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118"/>
       <c r="B118"/>
       <c r="J118"/>
       <c r="K118"/>
       <c r="N118"/>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119"/>
       <c r="B119"/>
       <c r="J119"/>
       <c r="K119"/>
       <c r="N119"/>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120"/>
       <c r="B120"/>
       <c r="J120"/>
       <c r="K120"/>
       <c r="N120"/>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121"/>
       <c r="B121"/>
       <c r="J121"/>
       <c r="K121"/>
       <c r="N121"/>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122"/>
       <c r="B122"/>
       <c r="J122"/>
       <c r="K122"/>
       <c r="N122"/>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123"/>
       <c r="B123"/>
       <c r="J123"/>
       <c r="K123"/>
       <c r="N123"/>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124"/>
       <c r="B124"/>
       <c r="J124"/>
       <c r="K124"/>
       <c r="N124"/>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125"/>
       <c r="B125"/>
       <c r="J125"/>
       <c r="K125"/>
       <c r="N125"/>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126"/>
       <c r="B126"/>
       <c r="J126"/>
       <c r="K126"/>
       <c r="N126"/>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127"/>
       <c r="B127"/>
       <c r="J127"/>
       <c r="K127"/>
       <c r="N127"/>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128"/>
       <c r="B128"/>
       <c r="J128"/>
       <c r="K128"/>
       <c r="N128"/>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129"/>
       <c r="B129"/>
       <c r="J129"/>
       <c r="K129"/>
       <c r="N129"/>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130"/>
       <c r="B130"/>
       <c r="J130"/>
       <c r="K130"/>
       <c r="N130"/>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131"/>
       <c r="B131"/>
       <c r="J131"/>
       <c r="K131"/>
       <c r="N131"/>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132"/>
       <c r="B132"/>
       <c r="J132"/>
       <c r="K132"/>
       <c r="N132"/>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133"/>
       <c r="B133"/>
       <c r="J133"/>
       <c r="K133"/>
       <c r="N133"/>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134"/>
       <c r="B134"/>
       <c r="J134"/>
       <c r="K134"/>
       <c r="N134"/>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135"/>
       <c r="B135"/>
       <c r="J135"/>
       <c r="K135"/>
       <c r="N135"/>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136"/>
       <c r="B136"/>
       <c r="J136"/>
       <c r="K136"/>
       <c r="N136"/>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137"/>
       <c r="B137"/>
       <c r="J137"/>
       <c r="K137"/>
       <c r="N137"/>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138"/>
       <c r="B138"/>
       <c r="J138"/>
       <c r="K138"/>
       <c r="N138"/>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139"/>
       <c r="B139"/>
       <c r="J139"/>
       <c r="K139"/>
       <c r="N139"/>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140"/>
       <c r="B140"/>
       <c r="J140"/>
       <c r="K140"/>
       <c r="N140"/>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141"/>
       <c r="B141"/>
       <c r="J141"/>
       <c r="K141"/>
       <c r="N141"/>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142"/>
       <c r="B142"/>
       <c r="J142"/>
       <c r="K142"/>
       <c r="N142"/>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143"/>
       <c r="B143"/>
       <c r="J143"/>
       <c r="K143"/>
       <c r="N143"/>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144"/>
       <c r="B144"/>
       <c r="J144"/>
       <c r="K144"/>
       <c r="N144"/>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145"/>
       <c r="B145"/>
       <c r="J145"/>
       <c r="K145"/>
       <c r="N145"/>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146"/>
       <c r="B146"/>
       <c r="J146"/>
       <c r="K146"/>
       <c r="N146"/>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147"/>
       <c r="B147"/>
       <c r="J147"/>
       <c r="K147"/>
       <c r="N147"/>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148"/>
       <c r="B148"/>
       <c r="J148"/>
       <c r="K148"/>
       <c r="N148"/>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149"/>
       <c r="B149"/>
       <c r="J149"/>
       <c r="K149"/>
       <c r="N149"/>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150"/>
       <c r="B150"/>
       <c r="J150"/>
       <c r="K150"/>
       <c r="N150"/>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151"/>
       <c r="B151"/>
       <c r="J151"/>
       <c r="K151"/>
       <c r="N151"/>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152"/>
       <c r="B152"/>
       <c r="J152"/>
       <c r="K152"/>
       <c r="N152"/>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153"/>
       <c r="B153"/>
       <c r="J153"/>
       <c r="K153"/>
       <c r="N153"/>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154"/>
       <c r="B154"/>
       <c r="J154"/>
       <c r="K154"/>
       <c r="N154"/>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155"/>
       <c r="B155"/>
       <c r="J155"/>
       <c r="K155"/>
       <c r="N155"/>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156"/>
       <c r="B156"/>
       <c r="J156"/>
       <c r="K156"/>
       <c r="N156"/>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157"/>
       <c r="B157"/>
       <c r="J157"/>
       <c r="K157"/>
       <c r="N157"/>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158"/>
       <c r="B158"/>
       <c r="J158"/>
       <c r="K158"/>
       <c r="N158"/>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A159"/>
       <c r="B159"/>
       <c r="J159"/>
       <c r="K159"/>
       <c r="N159"/>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A160"/>
       <c r="B160"/>
       <c r="J160"/>
       <c r="K160"/>
       <c r="N160"/>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A161"/>
       <c r="B161"/>
       <c r="J161"/>
       <c r="K161"/>
       <c r="N161"/>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A162"/>
       <c r="B162"/>
       <c r="J162"/>
       <c r="K162"/>
       <c r="N162"/>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A163"/>
       <c r="B163"/>
       <c r="J163"/>
       <c r="K163"/>
       <c r="N163"/>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A164"/>
       <c r="B164"/>
       <c r="J164"/>
       <c r="K164"/>
       <c r="N164"/>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A165"/>
       <c r="B165"/>
       <c r="J165"/>
       <c r="K165"/>
       <c r="N165"/>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A166"/>
       <c r="B166"/>
       <c r="J166"/>
       <c r="K166"/>
       <c r="N166"/>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A167"/>
       <c r="B167"/>
       <c r="J167"/>
       <c r="K167"/>
       <c r="N167"/>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A168"/>
       <c r="B168"/>
       <c r="J168"/>
       <c r="K168"/>
       <c r="N168"/>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A169"/>
       <c r="B169"/>
       <c r="J169"/>
       <c r="K169"/>
       <c r="N169"/>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A170"/>
       <c r="B170"/>
       <c r="J170"/>
       <c r="K170"/>
       <c r="N170"/>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A171"/>
       <c r="B171"/>
       <c r="J171"/>
       <c r="K171"/>
       <c r="N171"/>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A172"/>
       <c r="B172"/>
       <c r="J172"/>
       <c r="K172"/>
       <c r="N172"/>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A173"/>
       <c r="B173"/>
       <c r="J173"/>
       <c r="K173"/>
       <c r="N173"/>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A174"/>
       <c r="B174"/>
       <c r="J174"/>
       <c r="K174"/>
       <c r="N174"/>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A175"/>
       <c r="B175"/>
       <c r="J175"/>
       <c r="K175"/>
       <c r="N175"/>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A176"/>
       <c r="B176"/>
       <c r="J176"/>
       <c r="K176"/>
       <c r="N176"/>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A177"/>
       <c r="B177"/>
       <c r="J177"/>
       <c r="K177"/>
       <c r="N177"/>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A178"/>
       <c r="B178"/>
       <c r="J178"/>
       <c r="K178"/>
       <c r="N178"/>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A179"/>
       <c r="B179"/>
       <c r="J179"/>
       <c r="K179"/>
       <c r="N179"/>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A180"/>
       <c r="B180"/>
       <c r="J180"/>
       <c r="K180"/>
       <c r="N180"/>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A181"/>
       <c r="B181"/>
       <c r="J181"/>
       <c r="K181"/>
       <c r="N181"/>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A182"/>
       <c r="B182"/>
       <c r="J182"/>
       <c r="K182"/>
       <c r="N182"/>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A183"/>
       <c r="B183"/>
       <c r="J183"/>
       <c r="K183"/>
       <c r="N183"/>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A184"/>
       <c r="B184"/>
       <c r="J184"/>
       <c r="K184"/>
       <c r="N184"/>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A185"/>
       <c r="B185"/>
       <c r="J185"/>
       <c r="K185"/>
       <c r="N185"/>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A186"/>
       <c r="B186"/>
       <c r="J186"/>
       <c r="K186"/>
       <c r="N186"/>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A187"/>
       <c r="B187"/>
       <c r="J187"/>
       <c r="K187"/>
       <c r="N187"/>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A188"/>
       <c r="B188"/>
       <c r="J188"/>
       <c r="K188"/>
       <c r="N188"/>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A189"/>
       <c r="B189"/>
       <c r="J189"/>
       <c r="K189"/>
       <c r="N189"/>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A190"/>
       <c r="B190"/>
       <c r="J190"/>
       <c r="K190"/>
       <c r="N190"/>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A191"/>
       <c r="B191"/>
       <c r="J191"/>
       <c r="K191"/>
       <c r="N191"/>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A192"/>
       <c r="B192"/>
       <c r="J192"/>
       <c r="K192"/>
       <c r="N192"/>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A193"/>
       <c r="B193"/>
       <c r="J193"/>
       <c r="K193"/>
       <c r="N193"/>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A194"/>
       <c r="B194"/>
       <c r="J194"/>
       <c r="K194"/>
       <c r="N194"/>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A195"/>
       <c r="B195"/>
       <c r="J195"/>
       <c r="K195"/>
       <c r="N195"/>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A196"/>
       <c r="B196"/>
       <c r="J196"/>
       <c r="K196"/>
       <c r="N196"/>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A197"/>
       <c r="B197"/>
       <c r="J197"/>
       <c r="K197"/>
       <c r="N197"/>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A198"/>
       <c r="B198"/>
       <c r="J198"/>
       <c r="K198"/>
       <c r="N198"/>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A199"/>
       <c r="B199"/>
       <c r="J199"/>
       <c r="K199"/>
       <c r="N199"/>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A200"/>
       <c r="B200"/>
       <c r="J200"/>
       <c r="K200"/>
       <c r="N200"/>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A201"/>
       <c r="B201"/>
       <c r="J201"/>
       <c r="K201"/>
       <c r="N201"/>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A202"/>
       <c r="B202"/>
       <c r="J202"/>
       <c r="K202"/>
       <c r="N202"/>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A203"/>
       <c r="B203"/>
       <c r="J203"/>
       <c r="K203"/>
       <c r="N203"/>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A204"/>
       <c r="B204"/>
       <c r="J204"/>
       <c r="K204"/>
       <c r="N204"/>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A205"/>
       <c r="B205"/>
       <c r="J205"/>
       <c r="K205"/>
       <c r="N205"/>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A206"/>
       <c r="B206"/>
       <c r="J206"/>
       <c r="K206"/>
       <c r="N206"/>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A207"/>
       <c r="B207"/>
       <c r="J207"/>
       <c r="K207"/>
       <c r="N207"/>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A208"/>
       <c r="B208"/>
       <c r="J208"/>
       <c r="K208"/>
       <c r="N208"/>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A209"/>
       <c r="B209"/>
       <c r="J209"/>
       <c r="K209"/>
       <c r="N209"/>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210"/>
       <c r="B210"/>
       <c r="J210"/>
       <c r="K210"/>
       <c r="N210"/>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211"/>
       <c r="B211"/>
       <c r="J211"/>
       <c r="K211"/>
       <c r="N211"/>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A212"/>
       <c r="B212"/>
       <c r="J212"/>
       <c r="K212"/>
       <c r="N212"/>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213"/>
       <c r="B213"/>
       <c r="J213"/>
       <c r="K213"/>
       <c r="N213"/>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A214"/>
       <c r="B214"/>
       <c r="J214"/>
       <c r="K214"/>
       <c r="N214"/>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A215"/>
       <c r="B215"/>
       <c r="J215"/>
       <c r="K215"/>
       <c r="N215"/>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A216"/>
       <c r="B216"/>
       <c r="J216"/>
       <c r="K216"/>
       <c r="N216"/>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A217"/>
       <c r="B217"/>
       <c r="J217"/>
       <c r="K217"/>
       <c r="N217"/>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A218"/>
       <c r="B218"/>
       <c r="J218"/>
       <c r="K218"/>
       <c r="N218"/>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A219"/>
       <c r="B219"/>
       <c r="J219"/>
       <c r="K219"/>
       <c r="N219"/>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A220"/>
       <c r="B220"/>
       <c r="J220"/>
       <c r="K220"/>
       <c r="N220"/>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A221"/>
       <c r="B221"/>
       <c r="J221"/>
       <c r="K221"/>
       <c r="N221"/>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A222"/>
       <c r="B222"/>
       <c r="J222"/>
       <c r="K222"/>
       <c r="N222"/>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A223"/>
       <c r="B223"/>
       <c r="J223"/>
       <c r="K223"/>
       <c r="N223"/>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A224"/>
       <c r="B224"/>
       <c r="J224"/>
       <c r="K224"/>
       <c r="N224"/>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A225"/>
       <c r="B225"/>
       <c r="J225"/>
       <c r="K225"/>
       <c r="N225"/>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A226"/>
       <c r="B226"/>
       <c r="J226"/>
       <c r="K226"/>
       <c r="N226"/>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A227"/>
       <c r="B227"/>
       <c r="J227"/>
       <c r="K227"/>
       <c r="N227"/>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A228"/>
       <c r="B228"/>
       <c r="J228"/>
       <c r="K228"/>
       <c r="N228"/>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A229"/>
       <c r="B229"/>
       <c r="J229"/>
       <c r="K229"/>
       <c r="N229"/>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A230"/>
       <c r="B230"/>
       <c r="J230"/>
       <c r="K230"/>
       <c r="N230"/>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A231"/>
       <c r="B231"/>
       <c r="J231"/>
       <c r="K231"/>
       <c r="N231"/>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A232"/>
       <c r="B232"/>
       <c r="J232"/>
       <c r="K232"/>
       <c r="N232"/>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A233"/>
       <c r="B233"/>
       <c r="J233"/>
       <c r="K233"/>
       <c r="N233"/>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A234"/>
       <c r="B234"/>
       <c r="J234"/>
       <c r="K234"/>
       <c r="N234"/>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A235"/>
       <c r="B235"/>
       <c r="J235"/>
       <c r="K235"/>
       <c r="N235"/>
     </row>
+    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A236"/>
+      <c r="B236"/>
+      <c r="J236"/>
+      <c r="K236"/>
+      <c r="N236"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:T66" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T67" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Unit to Source
Added Unit of Measurement to Source
</commit_message>
<xml_diff>
--- a/BROMappings/Mapping en definitie BRO GLD.xlsx
+++ b/BROMappings/Mapping en definitie BRO GLD.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/trunk/BronDatamodel/BROMappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{BE372826-5466-43B2-95C7-E0F7EC2978EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{231EAFB2-03BE-48AB-B61B-443383F1B234}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{BE372826-5466-43B2-95C7-E0F7EC2978EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{457723EE-6752-45BD-925A-8C69040F6E01}"/>
   <bookViews>
-    <workbookView xWindow="33840" yWindow="4515" windowWidth="23040" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="264">
   <si>
     <t>Opmerking</t>
   </si>
@@ -669,9 +669,6 @@
     <t>Afgekeurd = NaN in values</t>
   </si>
   <si>
-    <t>Bevat TijdmeetwaardeReeks (DateTime en Value)</t>
-  </si>
-  <si>
     <t>Correcties</t>
   </si>
   <si>
@@ -811,6 +808,18 @@
   </si>
   <si>
     <t>Index van C.DATA.BRO.COM.List.QualityRegime</t>
+  </si>
+  <si>
+    <t>Bevat TijdmeetwaardeReeks (DateTime en RawValue), de gekeurde waarde (Value) wordt afgeleid uit de RawValue en Changes</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Reference level of measurement</t>
+  </si>
+  <si>
+    <t>Unit of measurement</t>
   </si>
 </sst>
 </file>
@@ -1241,14 +1250,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T236"/>
+  <dimension ref="A1:T237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3630" ySplit="570" topLeftCell="M1" activePane="bottomRight"/>
+      <pane xSplit="3630" ySplit="570" topLeftCell="J10" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59:XFD59"/>
+      <selection pane="bottomRight" activeCell="T59" sqref="T59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,22 +1375,22 @@
       </c>
       <c r="N2"/>
       <c r="O2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="R2" s="18" t="s">
         <v>175</v>
       </c>
       <c r="S2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="T2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -1418,19 +1427,19 @@
         <v>173</v>
       </c>
       <c r="P3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="R3" s="18" t="s">
         <v>175</v>
       </c>
       <c r="S3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="T3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -1464,22 +1473,22 @@
       </c>
       <c r="N4"/>
       <c r="O4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="R4" s="18" t="s">
         <v>175</v>
       </c>
       <c r="S4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="T4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1512,22 +1521,22 @@
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="R5" s="17" t="s">
         <v>175</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -1558,7 +1567,7 @@
       </c>
       <c r="N6"/>
       <c r="O6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P6" t="s">
         <v>174</v>
@@ -1567,7 +1576,7 @@
         <v>174</v>
       </c>
       <c r="R6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -1600,7 +1609,7 @@
         <v>49</v>
       </c>
       <c r="O7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P7" t="s">
         <v>176</v>
@@ -1660,13 +1669,13 @@
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" t="s">
         <v>244</v>
       </c>
-      <c r="D9" t="s">
-        <v>245</v>
-      </c>
       <c r="E9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
@@ -1681,19 +1690,19 @@
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N9" t="s">
         <v>51</v>
       </c>
       <c r="O9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>177</v>
@@ -1731,7 +1740,7 @@
         <v>52</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>181</v>
@@ -1740,13 +1749,13 @@
         <v>181</v>
       </c>
       <c r="R10" t="s">
+        <v>258</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -1779,7 +1788,7 @@
         <v>82</v>
       </c>
       <c r="O11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P11" t="s">
         <v>191</v>
@@ -1791,7 +1800,7 @@
         <v>183</v>
       </c>
       <c r="T11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1832,20 +1841,20 @@
         <v>196</v>
       </c>
       <c r="O12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R12" t="s">
         <v>184</v>
       </c>
       <c r="S12"/>
       <c r="T12" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2388,16 +2397,16 @@
         <v>173</v>
       </c>
       <c r="P25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="R25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="T25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2442,7 +2451,7 @@
       </c>
       <c r="S26"/>
       <c r="T26" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
@@ -2610,7 +2619,7 @@
         <v>108</v>
       </c>
       <c r="O30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P30" t="s">
         <v>211</v>
@@ -2821,7 +2830,7 @@
         <v>123</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P35" s="1" t="s">
         <v>190</v>
@@ -2830,7 +2839,7 @@
         <v>190</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
@@ -2845,7 +2854,7 @@
         <v>120</v>
       </c>
       <c r="E36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F36" t="s">
         <v>124</v>
@@ -2863,7 +2872,7 @@
         <v>127</v>
       </c>
       <c r="O36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P36" t="s">
         <v>194</v>
@@ -2946,7 +2955,7 @@
         <v>142</v>
       </c>
       <c r="O38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P38" t="s">
         <v>210</v>
@@ -2958,7 +2967,7 @@
         <v>184</v>
       </c>
       <c r="T38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
@@ -3437,19 +3446,19 @@
     </row>
     <row r="50" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="C50" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="D50" s="12" t="s">
+      <c r="E50" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="F50" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>239</v>
       </c>
       <c r="J50" s="13">
         <v>0</v>
@@ -3458,23 +3467,23 @@
         <v>172</v>
       </c>
       <c r="M50" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N50" s="14"/>
       <c r="O50" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P50" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q50" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R50" s="15" t="s">
         <v>182</v>
       </c>
       <c r="T50" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.3">
@@ -3516,13 +3525,13 @@
         <v>196</v>
       </c>
       <c r="O51" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R51" t="s">
         <v>183</v>
@@ -3567,19 +3576,19 @@
         <v>196</v>
       </c>
       <c r="O52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Q52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="R52" t="s">
         <v>184</v>
       </c>
       <c r="T52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.3">
@@ -3621,13 +3630,13 @@
         <v>196</v>
       </c>
       <c r="O53" t="s">
+        <v>217</v>
+      </c>
+      <c r="P53" t="s">
         <v>218</v>
       </c>
-      <c r="P53" t="s">
-        <v>219</v>
-      </c>
       <c r="Q53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R53" s="10" t="s">
         <v>200</v>
@@ -3673,7 +3682,7 @@
       </c>
       <c r="N54"/>
       <c r="O54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P54" t="s">
         <v>198</v>
@@ -3724,16 +3733,16 @@
         <v>196</v>
       </c>
       <c r="O55" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P55" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>249</v>
+      </c>
+      <c r="R55" t="s">
         <v>250</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>250</v>
-      </c>
-      <c r="R55" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.3">
@@ -3775,13 +3784,13 @@
         <v>196</v>
       </c>
       <c r="O56" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P56" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q56" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="R56" t="s">
         <v>182</v>
@@ -3827,19 +3836,19 @@
       </c>
       <c r="N57"/>
       <c r="O57" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P57" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Q57" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="R57" t="s">
         <v>178</v>
       </c>
       <c r="T57" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.3">
@@ -3882,17 +3891,20 @@
       </c>
       <c r="N58"/>
       <c r="O58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R58" t="s">
         <v>182</v>
       </c>
+      <c r="T58" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -3934,16 +3946,19 @@
       </c>
       <c r="N59"/>
       <c r="O59" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P59" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
       <c r="Q59" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
       <c r="R59" t="s">
-        <v>205</v>
+        <v>182</v>
+      </c>
+      <c r="T59" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.3">
@@ -3986,16 +4001,16 @@
       </c>
       <c r="N60"/>
       <c r="O60" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P60" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Q60" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="R60" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.3">
@@ -4038,16 +4053,16 @@
       </c>
       <c r="N61"/>
       <c r="O61" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P61" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="Q61" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="R61" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.3">
@@ -4090,16 +4105,16 @@
       </c>
       <c r="N62"/>
       <c r="O62" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P62" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Q62" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R62" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.3">
@@ -4142,19 +4157,16 @@
       </c>
       <c r="N63"/>
       <c r="O63" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P63" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="Q63" t="s">
-        <v>222</v>
-      </c>
-      <c r="R63" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="T63" t="s">
-        <v>213</v>
+        <v>208</v>
+      </c>
+      <c r="R63" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.3">
@@ -4197,22 +4209,22 @@
       </c>
       <c r="N64"/>
       <c r="O64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P64" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="Q64" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="R64" s="10" t="s">
         <v>200</v>
       </c>
       <c r="T64" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>179</v>
       </c>
@@ -4252,19 +4264,22 @@
       </c>
       <c r="N65"/>
       <c r="O65" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P65" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="Q65" t="s">
-        <v>201</v>
-      </c>
-      <c r="R65" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="R65" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="T65" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>179</v>
       </c>
@@ -4304,19 +4319,19 @@
       </c>
       <c r="N66"/>
       <c r="O66" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P66" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="Q66" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="R66" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>179</v>
       </c>
@@ -4356,267 +4371,1255 @@
       </c>
       <c r="N67"/>
       <c r="O67" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P67" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>204</v>
+      </c>
+      <c r="R67" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>179</v>
+      </c>
+      <c r="B68"/>
+      <c r="C68" t="s">
+        <v>179</v>
+      </c>
+      <c r="D68" t="s">
+        <v>179</v>
+      </c>
+      <c r="E68" t="s">
+        <v>179</v>
+      </c>
+      <c r="F68" t="s">
+        <v>179</v>
+      </c>
+      <c r="G68" t="s">
+        <v>179</v>
+      </c>
+      <c r="H68" t="s">
+        <v>179</v>
+      </c>
+      <c r="I68" t="s">
+        <v>179</v>
+      </c>
+      <c r="J68" t="s">
+        <v>179</v>
+      </c>
+      <c r="K68" t="s">
+        <v>179</v>
+      </c>
+      <c r="L68" t="s">
+        <v>179</v>
+      </c>
+      <c r="M68" t="s">
+        <v>179</v>
+      </c>
+      <c r="N68"/>
+      <c r="O68" t="s">
+        <v>222</v>
+      </c>
+      <c r="P68" t="s">
         <v>203</v>
       </c>
-      <c r="Q67" t="s">
+      <c r="Q68" t="s">
         <v>203</v>
       </c>
-      <c r="R67" t="s">
+      <c r="R68" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="J68"/>
-      <c r="K68"/>
-      <c r="N68"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69"/>
       <c r="J69"/>
       <c r="K69"/>
       <c r="N69"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70"/>
       <c r="J70"/>
       <c r="K70"/>
       <c r="N70"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71"/>
       <c r="J71"/>
       <c r="K71"/>
       <c r="N71"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72"/>
       <c r="J72"/>
       <c r="K72"/>
       <c r="N72"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73"/>
       <c r="J73"/>
       <c r="K73"/>
       <c r="N73"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74"/>
       <c r="J74"/>
       <c r="K74"/>
       <c r="N74"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75"/>
       <c r="J75"/>
       <c r="K75"/>
       <c r="N75"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="B76"/>
       <c r="J76"/>
       <c r="K76"/>
       <c r="N76"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="B77"/>
       <c r="J77"/>
       <c r="K77"/>
       <c r="N77"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="B78"/>
       <c r="J78"/>
       <c r="K78"/>
       <c r="N78"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="B79"/>
       <c r="J79"/>
       <c r="K79"/>
       <c r="N79"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="J80"/>
       <c r="K80"/>
       <c r="N80"/>
     </row>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="131" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="132" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="133" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="134" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="135" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="136" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="137" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="138" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="139" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="140" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="141" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="142" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="143" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="144" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="145" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="146" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="147" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="148" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="149" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="150" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="151" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="152" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="153" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="154" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="155" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="156" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="157" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="158" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="159" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="160" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="161" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="162" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="163" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="164" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="165" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="166" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="167" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="168" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="169" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="170" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="171" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="172" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="173" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="174" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="175" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="176" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="177" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="178" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="179" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="180" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="181" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="182" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="183" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="184" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="185" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="186" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="187" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="188" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="189" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="190" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="191" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="192" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="193" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="194" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="195" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="196" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="197" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="198" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="199" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="200" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="201" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="202" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="203" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="204" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="205" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="206" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="207" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="208" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="209" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="210" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="211" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="212" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="213" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="214" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="215" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="216" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="217" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="218" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="219" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="220" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="221" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="222" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="223" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="224" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="225" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="226" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="227" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="228" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="229" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="230" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="231" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="232" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="233" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="234" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="235" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="236" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A81"/>
+      <c r="B81"/>
+      <c r="J81"/>
+      <c r="K81"/>
+      <c r="N81"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A82"/>
+      <c r="B82"/>
+      <c r="J82"/>
+      <c r="K82"/>
+      <c r="N82"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A83"/>
+      <c r="B83"/>
+      <c r="J83"/>
+      <c r="K83"/>
+      <c r="N83"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A84"/>
+      <c r="B84"/>
+      <c r="J84"/>
+      <c r="K84"/>
+      <c r="N84"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A85"/>
+      <c r="B85"/>
+      <c r="J85"/>
+      <c r="K85"/>
+      <c r="N85"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="J86"/>
+      <c r="K86"/>
+      <c r="N86"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A87"/>
+      <c r="B87"/>
+      <c r="J87"/>
+      <c r="K87"/>
+      <c r="N87"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A88"/>
+      <c r="B88"/>
+      <c r="J88"/>
+      <c r="K88"/>
+      <c r="N88"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A89"/>
+      <c r="B89"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="N89"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A90"/>
+      <c r="B90"/>
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="N90"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A91"/>
+      <c r="B91"/>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="N91"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A92"/>
+      <c r="B92"/>
+      <c r="J92"/>
+      <c r="K92"/>
+      <c r="N92"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A93"/>
+      <c r="B93"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="N93"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="N94"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="N95"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A96"/>
+      <c r="B96"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="N96"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A97"/>
+      <c r="B97"/>
+      <c r="J97"/>
+      <c r="K97"/>
+      <c r="N97"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A98"/>
+      <c r="B98"/>
+      <c r="J98"/>
+      <c r="K98"/>
+      <c r="N98"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A99"/>
+      <c r="B99"/>
+      <c r="J99"/>
+      <c r="K99"/>
+      <c r="N99"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A100"/>
+      <c r="B100"/>
+      <c r="J100"/>
+      <c r="K100"/>
+      <c r="N100"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A101"/>
+      <c r="B101"/>
+      <c r="J101"/>
+      <c r="K101"/>
+      <c r="N101"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A102"/>
+      <c r="B102"/>
+      <c r="J102"/>
+      <c r="K102"/>
+      <c r="N102"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A103"/>
+      <c r="B103"/>
+      <c r="J103"/>
+      <c r="K103"/>
+      <c r="N103"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A104"/>
+      <c r="B104"/>
+      <c r="J104"/>
+      <c r="K104"/>
+      <c r="N104"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A105"/>
+      <c r="B105"/>
+      <c r="J105"/>
+      <c r="K105"/>
+      <c r="N105"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A106"/>
+      <c r="B106"/>
+      <c r="J106"/>
+      <c r="K106"/>
+      <c r="N106"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A107"/>
+      <c r="B107"/>
+      <c r="J107"/>
+      <c r="K107"/>
+      <c r="N107"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A108"/>
+      <c r="B108"/>
+      <c r="J108"/>
+      <c r="K108"/>
+      <c r="N108"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A109"/>
+      <c r="B109"/>
+      <c r="J109"/>
+      <c r="K109"/>
+      <c r="N109"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A110"/>
+      <c r="B110"/>
+      <c r="J110"/>
+      <c r="K110"/>
+      <c r="N110"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A111"/>
+      <c r="B111"/>
+      <c r="J111"/>
+      <c r="K111"/>
+      <c r="N111"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A112"/>
+      <c r="B112"/>
+      <c r="J112"/>
+      <c r="K112"/>
+      <c r="N112"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A113"/>
+      <c r="B113"/>
+      <c r="J113"/>
+      <c r="K113"/>
+      <c r="N113"/>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A114"/>
+      <c r="B114"/>
+      <c r="J114"/>
+      <c r="K114"/>
+      <c r="N114"/>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A115"/>
+      <c r="B115"/>
+      <c r="J115"/>
+      <c r="K115"/>
+      <c r="N115"/>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A116"/>
+      <c r="B116"/>
+      <c r="J116"/>
+      <c r="K116"/>
+      <c r="N116"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A117"/>
+      <c r="B117"/>
+      <c r="J117"/>
+      <c r="K117"/>
+      <c r="N117"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A118"/>
+      <c r="B118"/>
+      <c r="J118"/>
+      <c r="K118"/>
+      <c r="N118"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A119"/>
+      <c r="B119"/>
+      <c r="J119"/>
+      <c r="K119"/>
+      <c r="N119"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A120"/>
+      <c r="B120"/>
+      <c r="J120"/>
+      <c r="K120"/>
+      <c r="N120"/>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A121"/>
+      <c r="B121"/>
+      <c r="J121"/>
+      <c r="K121"/>
+      <c r="N121"/>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A122"/>
+      <c r="B122"/>
+      <c r="J122"/>
+      <c r="K122"/>
+      <c r="N122"/>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A123"/>
+      <c r="B123"/>
+      <c r="J123"/>
+      <c r="K123"/>
+      <c r="N123"/>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A124"/>
+      <c r="B124"/>
+      <c r="J124"/>
+      <c r="K124"/>
+      <c r="N124"/>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A125"/>
+      <c r="B125"/>
+      <c r="J125"/>
+      <c r="K125"/>
+      <c r="N125"/>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A126"/>
+      <c r="B126"/>
+      <c r="J126"/>
+      <c r="K126"/>
+      <c r="N126"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A127"/>
+      <c r="B127"/>
+      <c r="J127"/>
+      <c r="K127"/>
+      <c r="N127"/>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A128"/>
+      <c r="B128"/>
+      <c r="J128"/>
+      <c r="K128"/>
+      <c r="N128"/>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A129"/>
+      <c r="B129"/>
+      <c r="J129"/>
+      <c r="K129"/>
+      <c r="N129"/>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A130"/>
+      <c r="B130"/>
+      <c r="J130"/>
+      <c r="K130"/>
+      <c r="N130"/>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A131"/>
+      <c r="B131"/>
+      <c r="J131"/>
+      <c r="K131"/>
+      <c r="N131"/>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A132"/>
+      <c r="B132"/>
+      <c r="J132"/>
+      <c r="K132"/>
+      <c r="N132"/>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A133"/>
+      <c r="B133"/>
+      <c r="J133"/>
+      <c r="K133"/>
+      <c r="N133"/>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A134"/>
+      <c r="B134"/>
+      <c r="J134"/>
+      <c r="K134"/>
+      <c r="N134"/>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A135"/>
+      <c r="B135"/>
+      <c r="J135"/>
+      <c r="K135"/>
+      <c r="N135"/>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A136"/>
+      <c r="B136"/>
+      <c r="J136"/>
+      <c r="K136"/>
+      <c r="N136"/>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A137"/>
+      <c r="B137"/>
+      <c r="J137"/>
+      <c r="K137"/>
+      <c r="N137"/>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A138"/>
+      <c r="B138"/>
+      <c r="J138"/>
+      <c r="K138"/>
+      <c r="N138"/>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A139"/>
+      <c r="B139"/>
+      <c r="J139"/>
+      <c r="K139"/>
+      <c r="N139"/>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A140"/>
+      <c r="B140"/>
+      <c r="J140"/>
+      <c r="K140"/>
+      <c r="N140"/>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A141"/>
+      <c r="B141"/>
+      <c r="J141"/>
+      <c r="K141"/>
+      <c r="N141"/>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A142"/>
+      <c r="B142"/>
+      <c r="J142"/>
+      <c r="K142"/>
+      <c r="N142"/>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A143"/>
+      <c r="B143"/>
+      <c r="J143"/>
+      <c r="K143"/>
+      <c r="N143"/>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A144"/>
+      <c r="B144"/>
+      <c r="J144"/>
+      <c r="K144"/>
+      <c r="N144"/>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A145"/>
+      <c r="B145"/>
+      <c r="J145"/>
+      <c r="K145"/>
+      <c r="N145"/>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A146"/>
+      <c r="B146"/>
+      <c r="J146"/>
+      <c r="K146"/>
+      <c r="N146"/>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A147"/>
+      <c r="B147"/>
+      <c r="J147"/>
+      <c r="K147"/>
+      <c r="N147"/>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A148"/>
+      <c r="B148"/>
+      <c r="J148"/>
+      <c r="K148"/>
+      <c r="N148"/>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A149"/>
+      <c r="B149"/>
+      <c r="J149"/>
+      <c r="K149"/>
+      <c r="N149"/>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A150"/>
+      <c r="B150"/>
+      <c r="J150"/>
+      <c r="K150"/>
+      <c r="N150"/>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A151"/>
+      <c r="B151"/>
+      <c r="J151"/>
+      <c r="K151"/>
+      <c r="N151"/>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A152"/>
+      <c r="B152"/>
+      <c r="J152"/>
+      <c r="K152"/>
+      <c r="N152"/>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A153"/>
+      <c r="B153"/>
+      <c r="J153"/>
+      <c r="K153"/>
+      <c r="N153"/>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A154"/>
+      <c r="B154"/>
+      <c r="J154"/>
+      <c r="K154"/>
+      <c r="N154"/>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A155"/>
+      <c r="B155"/>
+      <c r="J155"/>
+      <c r="K155"/>
+      <c r="N155"/>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A156"/>
+      <c r="B156"/>
+      <c r="J156"/>
+      <c r="K156"/>
+      <c r="N156"/>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A157"/>
+      <c r="B157"/>
+      <c r="J157"/>
+      <c r="K157"/>
+      <c r="N157"/>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A158"/>
+      <c r="B158"/>
+      <c r="J158"/>
+      <c r="K158"/>
+      <c r="N158"/>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A159"/>
+      <c r="B159"/>
+      <c r="J159"/>
+      <c r="K159"/>
+      <c r="N159"/>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A160"/>
+      <c r="B160"/>
+      <c r="J160"/>
+      <c r="K160"/>
+      <c r="N160"/>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A161"/>
+      <c r="B161"/>
+      <c r="J161"/>
+      <c r="K161"/>
+      <c r="N161"/>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A162"/>
+      <c r="B162"/>
+      <c r="J162"/>
+      <c r="K162"/>
+      <c r="N162"/>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A163"/>
+      <c r="B163"/>
+      <c r="J163"/>
+      <c r="K163"/>
+      <c r="N163"/>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A164"/>
+      <c r="B164"/>
+      <c r="J164"/>
+      <c r="K164"/>
+      <c r="N164"/>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A165"/>
+      <c r="B165"/>
+      <c r="J165"/>
+      <c r="K165"/>
+      <c r="N165"/>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A166"/>
+      <c r="B166"/>
+      <c r="J166"/>
+      <c r="K166"/>
+      <c r="N166"/>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A167"/>
+      <c r="B167"/>
+      <c r="J167"/>
+      <c r="K167"/>
+      <c r="N167"/>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A168"/>
+      <c r="B168"/>
+      <c r="J168"/>
+      <c r="K168"/>
+      <c r="N168"/>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A169"/>
+      <c r="B169"/>
+      <c r="J169"/>
+      <c r="K169"/>
+      <c r="N169"/>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A170"/>
+      <c r="B170"/>
+      <c r="J170"/>
+      <c r="K170"/>
+      <c r="N170"/>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A171"/>
+      <c r="B171"/>
+      <c r="J171"/>
+      <c r="K171"/>
+      <c r="N171"/>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A172"/>
+      <c r="B172"/>
+      <c r="J172"/>
+      <c r="K172"/>
+      <c r="N172"/>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A173"/>
+      <c r="B173"/>
+      <c r="J173"/>
+      <c r="K173"/>
+      <c r="N173"/>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A174"/>
+      <c r="B174"/>
+      <c r="J174"/>
+      <c r="K174"/>
+      <c r="N174"/>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A175"/>
+      <c r="B175"/>
+      <c r="J175"/>
+      <c r="K175"/>
+      <c r="N175"/>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A176"/>
+      <c r="B176"/>
+      <c r="J176"/>
+      <c r="K176"/>
+      <c r="N176"/>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A177"/>
+      <c r="B177"/>
+      <c r="J177"/>
+      <c r="K177"/>
+      <c r="N177"/>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A178"/>
+      <c r="B178"/>
+      <c r="J178"/>
+      <c r="K178"/>
+      <c r="N178"/>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A179"/>
+      <c r="B179"/>
+      <c r="J179"/>
+      <c r="K179"/>
+      <c r="N179"/>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A180"/>
+      <c r="B180"/>
+      <c r="J180"/>
+      <c r="K180"/>
+      <c r="N180"/>
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A181"/>
+      <c r="B181"/>
+      <c r="J181"/>
+      <c r="K181"/>
+      <c r="N181"/>
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A182"/>
+      <c r="B182"/>
+      <c r="J182"/>
+      <c r="K182"/>
+      <c r="N182"/>
+    </row>
+    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A183"/>
+      <c r="B183"/>
+      <c r="J183"/>
+      <c r="K183"/>
+      <c r="N183"/>
+    </row>
+    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A184"/>
+      <c r="B184"/>
+      <c r="J184"/>
+      <c r="K184"/>
+      <c r="N184"/>
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A185"/>
+      <c r="B185"/>
+      <c r="J185"/>
+      <c r="K185"/>
+      <c r="N185"/>
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A186"/>
+      <c r="B186"/>
+      <c r="J186"/>
+      <c r="K186"/>
+      <c r="N186"/>
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A187"/>
+      <c r="B187"/>
+      <c r="J187"/>
+      <c r="K187"/>
+      <c r="N187"/>
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A188"/>
+      <c r="B188"/>
+      <c r="J188"/>
+      <c r="K188"/>
+      <c r="N188"/>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A189"/>
+      <c r="B189"/>
+      <c r="J189"/>
+      <c r="K189"/>
+      <c r="N189"/>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A190"/>
+      <c r="B190"/>
+      <c r="J190"/>
+      <c r="K190"/>
+      <c r="N190"/>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A191"/>
+      <c r="B191"/>
+      <c r="J191"/>
+      <c r="K191"/>
+      <c r="N191"/>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A192"/>
+      <c r="B192"/>
+      <c r="J192"/>
+      <c r="K192"/>
+      <c r="N192"/>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A193"/>
+      <c r="B193"/>
+      <c r="J193"/>
+      <c r="K193"/>
+      <c r="N193"/>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A194"/>
+      <c r="B194"/>
+      <c r="J194"/>
+      <c r="K194"/>
+      <c r="N194"/>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A195"/>
+      <c r="B195"/>
+      <c r="J195"/>
+      <c r="K195"/>
+      <c r="N195"/>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A196"/>
+      <c r="B196"/>
+      <c r="J196"/>
+      <c r="K196"/>
+      <c r="N196"/>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A197"/>
+      <c r="B197"/>
+      <c r="J197"/>
+      <c r="K197"/>
+      <c r="N197"/>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A198"/>
+      <c r="B198"/>
+      <c r="J198"/>
+      <c r="K198"/>
+      <c r="N198"/>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A199"/>
+      <c r="B199"/>
+      <c r="J199"/>
+      <c r="K199"/>
+      <c r="N199"/>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A200"/>
+      <c r="B200"/>
+      <c r="J200"/>
+      <c r="K200"/>
+      <c r="N200"/>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A201"/>
+      <c r="B201"/>
+      <c r="J201"/>
+      <c r="K201"/>
+      <c r="N201"/>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A202"/>
+      <c r="B202"/>
+      <c r="J202"/>
+      <c r="K202"/>
+      <c r="N202"/>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A203"/>
+      <c r="B203"/>
+      <c r="J203"/>
+      <c r="K203"/>
+      <c r="N203"/>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A204"/>
+      <c r="B204"/>
+      <c r="J204"/>
+      <c r="K204"/>
+      <c r="N204"/>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A205"/>
+      <c r="B205"/>
+      <c r="J205"/>
+      <c r="K205"/>
+      <c r="N205"/>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A206"/>
+      <c r="B206"/>
+      <c r="J206"/>
+      <c r="K206"/>
+      <c r="N206"/>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A207"/>
+      <c r="B207"/>
+      <c r="J207"/>
+      <c r="K207"/>
+      <c r="N207"/>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A208"/>
+      <c r="B208"/>
+      <c r="J208"/>
+      <c r="K208"/>
+      <c r="N208"/>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A209"/>
+      <c r="B209"/>
+      <c r="J209"/>
+      <c r="K209"/>
+      <c r="N209"/>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A210"/>
+      <c r="B210"/>
+      <c r="J210"/>
+      <c r="K210"/>
+      <c r="N210"/>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A211"/>
+      <c r="B211"/>
+      <c r="J211"/>
+      <c r="K211"/>
+      <c r="N211"/>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A212"/>
+      <c r="B212"/>
+      <c r="J212"/>
+      <c r="K212"/>
+      <c r="N212"/>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A213"/>
+      <c r="B213"/>
+      <c r="J213"/>
+      <c r="K213"/>
+      <c r="N213"/>
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A214"/>
+      <c r="B214"/>
+      <c r="J214"/>
+      <c r="K214"/>
+      <c r="N214"/>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A215"/>
+      <c r="B215"/>
+      <c r="J215"/>
+      <c r="K215"/>
+      <c r="N215"/>
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A216"/>
+      <c r="B216"/>
+      <c r="J216"/>
+      <c r="K216"/>
+      <c r="N216"/>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A217"/>
+      <c r="B217"/>
+      <c r="J217"/>
+      <c r="K217"/>
+      <c r="N217"/>
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A218"/>
+      <c r="B218"/>
+      <c r="J218"/>
+      <c r="K218"/>
+      <c r="N218"/>
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A219"/>
+      <c r="B219"/>
+      <c r="J219"/>
+      <c r="K219"/>
+      <c r="N219"/>
+    </row>
+    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A220"/>
+      <c r="B220"/>
+      <c r="J220"/>
+      <c r="K220"/>
+      <c r="N220"/>
+    </row>
+    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A221"/>
+      <c r="B221"/>
+      <c r="J221"/>
+      <c r="K221"/>
+      <c r="N221"/>
+    </row>
+    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A222"/>
+      <c r="B222"/>
+      <c r="J222"/>
+      <c r="K222"/>
+      <c r="N222"/>
+    </row>
+    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A223"/>
+      <c r="B223"/>
+      <c r="J223"/>
+      <c r="K223"/>
+      <c r="N223"/>
+    </row>
+    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A224"/>
+      <c r="B224"/>
+      <c r="J224"/>
+      <c r="K224"/>
+      <c r="N224"/>
+    </row>
+    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A225"/>
+      <c r="B225"/>
+      <c r="J225"/>
+      <c r="K225"/>
+      <c r="N225"/>
+    </row>
+    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A226"/>
+      <c r="B226"/>
+      <c r="J226"/>
+      <c r="K226"/>
+      <c r="N226"/>
+    </row>
+    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A227"/>
+      <c r="B227"/>
+      <c r="J227"/>
+      <c r="K227"/>
+      <c r="N227"/>
+    </row>
+    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A228"/>
+      <c r="B228"/>
+      <c r="J228"/>
+      <c r="K228"/>
+      <c r="N228"/>
+    </row>
+    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A229"/>
+      <c r="B229"/>
+      <c r="J229"/>
+      <c r="K229"/>
+      <c r="N229"/>
+    </row>
+    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A230"/>
+      <c r="B230"/>
+      <c r="J230"/>
+      <c r="K230"/>
+      <c r="N230"/>
+    </row>
+    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A231"/>
+      <c r="B231"/>
+      <c r="J231"/>
+      <c r="K231"/>
+      <c r="N231"/>
+    </row>
+    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A232"/>
+      <c r="B232"/>
+      <c r="J232"/>
+      <c r="K232"/>
+      <c r="N232"/>
+    </row>
+    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A233"/>
+      <c r="B233"/>
+      <c r="J233"/>
+      <c r="K233"/>
+      <c r="N233"/>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A234"/>
+      <c r="B234"/>
+      <c r="J234"/>
+      <c r="K234"/>
+      <c r="N234"/>
+    </row>
+    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A235"/>
+      <c r="B235"/>
+      <c r="J235"/>
+      <c r="K235"/>
+      <c r="N235"/>
+    </row>
+    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A236"/>
+      <c r="B236"/>
+      <c r="J236"/>
+      <c r="K236"/>
+      <c r="N236"/>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A237"/>
+      <c r="B237"/>
+      <c r="J237"/>
+      <c r="K237"/>
+      <c r="N237"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:T67" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T68" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Suppletion SourceDatatype and correction EventDate
Column SourceDatatype is suppleted, EventDate is now corrected in DateTime for all objects
</commit_message>
<xml_diff>
--- a/BROMappings/Mapping en definitie BRO GLD.xlsx
+++ b/BROMappings/Mapping en definitie BRO GLD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/trunk/BronDatamodel/BROMappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{BE372826-5466-43B2-95C7-E0F7EC2978EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{457723EE-6752-45BD-925A-8C69040F6E01}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{BE372826-5466-43B2-95C7-E0F7EC2978EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9818DFA3-33ED-4171-A15C-D0C028A1FD56}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="267">
   <si>
     <t>Opmerking</t>
   </si>
@@ -786,9 +786,6 @@
     <t>LoggerBrand</t>
   </si>
   <si>
-    <t>EventDate</t>
-  </si>
-  <si>
     <t>Lokaal (bron-)ID, voor relaties met andere objecten, objecten zonder BRO-ID , willekeurige brondataselectie</t>
   </si>
   <si>
@@ -820,6 +817,18 @@
   </si>
   <si>
     <t>Unit of measurement</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>[DateTime]</t>
+  </si>
+  <si>
+    <t>[JaNeeOnbekend]</t>
+  </si>
+  <si>
+    <t>[m+NAP]</t>
   </si>
 </sst>
 </file>
@@ -851,21 +860,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -911,22 +914,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -947,15 +939,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1253,36 +1236,36 @@
   <dimension ref="A1:T237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3630" ySplit="570" topLeftCell="J10" activePane="bottomRight"/>
-      <selection sqref="A1:A1048576"/>
+      <pane xSplit="5820" ySplit="576" topLeftCell="P1" activePane="bottomLeft"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59:XFD59"/>
-      <selection pane="bottomRight" activeCell="T59" sqref="T59"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="60.5546875" style="8" customWidth="1"/>
-    <col min="15" max="17" width="25.33203125" customWidth="1"/>
-    <col min="18" max="18" width="26.33203125" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="77.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.5703125" style="8" customWidth="1"/>
+    <col min="15" max="17" width="25.28515625" customWidth="1"/>
+    <col min="18" max="18" width="26.28515625" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="77.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1344,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>179</v>
       </c>
@@ -1361,6 +1344,15 @@
       <c r="F2" t="s">
         <v>179</v>
       </c>
+      <c r="G2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I2" t="s">
+        <v>179</v>
+      </c>
       <c r="J2" s="2" t="s">
         <v>196</v>
       </c>
@@ -1373,27 +1365,29 @@
       <c r="M2" t="s">
         <v>196</v>
       </c>
-      <c r="N2"/>
+      <c r="N2" t="s">
+        <v>179</v>
+      </c>
       <c r="O2" t="s">
         <v>216</v>
       </c>
       <c r="P2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q2" t="s">
-        <v>254</v>
-      </c>
-      <c r="R2" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="R2" s="13" t="s">
         <v>175</v>
       </c>
       <c r="S2" t="s">
         <v>219</v>
       </c>
       <c r="T2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -1410,6 +1404,15 @@
       <c r="F3" t="s">
         <v>179</v>
       </c>
+      <c r="G3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I3" t="s">
+        <v>179</v>
+      </c>
       <c r="J3" s="2" t="s">
         <v>196</v>
       </c>
@@ -1422,27 +1425,29 @@
       <c r="M3" t="s">
         <v>196</v>
       </c>
-      <c r="N3"/>
+      <c r="N3" t="s">
+        <v>179</v>
+      </c>
       <c r="O3" t="s">
         <v>173</v>
       </c>
       <c r="P3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q3" t="s">
-        <v>257</v>
-      </c>
-      <c r="R3" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="R3" s="13" t="s">
         <v>175</v>
       </c>
       <c r="S3" t="s">
         <v>219</v>
       </c>
       <c r="T3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -1459,6 +1464,15 @@
       <c r="F4" t="s">
         <v>179</v>
       </c>
+      <c r="G4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I4" t="s">
+        <v>179</v>
+      </c>
       <c r="J4" s="2" t="s">
         <v>196</v>
       </c>
@@ -1471,27 +1485,29 @@
       <c r="M4" t="s">
         <v>196</v>
       </c>
-      <c r="N4"/>
+      <c r="N4" t="s">
+        <v>179</v>
+      </c>
       <c r="O4" t="s">
         <v>222</v>
       </c>
       <c r="P4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q4" t="s">
-        <v>254</v>
-      </c>
-      <c r="R4" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>175</v>
       </c>
       <c r="S4" t="s">
         <v>219</v>
       </c>
       <c r="T4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>179</v>
       </c>
@@ -1507,6 +1523,15 @@
       <c r="F5" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="J5" s="11" t="s">
         <v>196</v>
       </c>
@@ -1519,27 +1544,29 @@
       <c r="M5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="N5" s="16"/>
+      <c r="N5" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="O5" s="1" t="s">
         <v>217</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="R5" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="R5" s="12" t="s">
         <v>175</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>219</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>185</v>
       </c>
@@ -1556,6 +1583,9 @@
       <c r="F6" t="s">
         <v>27</v>
       </c>
+      <c r="G6" t="s">
+        <v>215</v>
+      </c>
       <c r="H6" t="s">
         <v>53</v>
       </c>
@@ -1579,7 +1609,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>185</v>
       </c>
@@ -1596,6 +1626,9 @@
       <c r="F7" t="s">
         <v>23</v>
       </c>
+      <c r="G7" t="s">
+        <v>177</v>
+      </c>
       <c r="H7" t="s">
         <v>32</v>
       </c>
@@ -1621,7 +1654,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -1638,6 +1671,9 @@
       <c r="F8" t="s">
         <v>26</v>
       </c>
+      <c r="G8" t="s">
+        <v>178</v>
+      </c>
       <c r="H8" t="s">
         <v>33</v>
       </c>
@@ -1663,7 +1699,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -1680,6 +1716,9 @@
       <c r="F9" t="s">
         <v>38</v>
       </c>
+      <c r="G9" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="H9" t="s">
         <v>32</v>
       </c>
@@ -1711,7 +1750,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>185</v>
       </c>
@@ -1727,6 +1766,9 @@
       <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="G10" t="s">
+        <v>257</v>
+      </c>
       <c r="H10" s="1" t="s">
         <v>34</v>
       </c>
@@ -1749,16 +1791,16 @@
         <v>181</v>
       </c>
       <c r="R10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>219</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>186</v>
       </c>
@@ -1775,6 +1817,9 @@
       <c r="F11" t="s">
         <v>57</v>
       </c>
+      <c r="G11" t="s">
+        <v>264</v>
+      </c>
       <c r="H11" t="s">
         <v>94</v>
       </c>
@@ -1803,7 +1848,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>179</v>
       </c>
@@ -1818,6 +1863,9 @@
       </c>
       <c r="F12" s="1" t="s">
         <v>179</v>
+      </c>
+      <c r="G12" t="s">
+        <v>184</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>196</v>
@@ -1857,7 +1905,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>186</v>
       </c>
@@ -1874,6 +1922,9 @@
       <c r="F13" t="s">
         <v>58</v>
       </c>
+      <c r="G13" t="s">
+        <v>182</v>
+      </c>
       <c r="H13" t="s">
         <v>34</v>
       </c>
@@ -1899,7 +1950,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>186</v>
       </c>
@@ -1916,6 +1967,9 @@
       <c r="F14" t="s">
         <v>59</v>
       </c>
+      <c r="G14" t="s">
+        <v>264</v>
+      </c>
       <c r="H14" t="s">
         <v>94</v>
       </c>
@@ -1944,7 +1998,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>186</v>
       </c>
@@ -1961,6 +2015,9 @@
       <c r="F15" t="s">
         <v>60</v>
       </c>
+      <c r="G15" t="s">
+        <v>264</v>
+      </c>
       <c r="H15" t="s">
         <v>94</v>
       </c>
@@ -1986,7 +2043,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>186</v>
       </c>
@@ -2003,6 +2060,9 @@
       <c r="F16" t="s">
         <v>61</v>
       </c>
+      <c r="G16" t="s">
+        <v>182</v>
+      </c>
       <c r="H16" t="s">
         <v>34</v>
       </c>
@@ -2028,7 +2088,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>186</v>
       </c>
@@ -2045,6 +2105,9 @@
       <c r="F17" t="s">
         <v>62</v>
       </c>
+      <c r="G17" t="s">
+        <v>264</v>
+      </c>
       <c r="H17" t="s">
         <v>94</v>
       </c>
@@ -2070,7 +2133,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>186</v>
       </c>
@@ -2087,6 +2150,9 @@
       <c r="F18" t="s">
         <v>63</v>
       </c>
+      <c r="G18" t="s">
+        <v>182</v>
+      </c>
       <c r="H18" t="s">
         <v>34</v>
       </c>
@@ -2112,7 +2178,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>186</v>
       </c>
@@ -2129,6 +2195,9 @@
       <c r="F19" t="s">
         <v>64</v>
       </c>
+      <c r="G19" t="s">
+        <v>264</v>
+      </c>
       <c r="H19" t="s">
         <v>94</v>
       </c>
@@ -2154,7 +2223,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -2171,6 +2240,9 @@
       <c r="F20" t="s">
         <v>65</v>
       </c>
+      <c r="G20" t="s">
+        <v>182</v>
+      </c>
       <c r="H20" t="s">
         <v>34</v>
       </c>
@@ -2196,7 +2268,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>186</v>
       </c>
@@ -2213,6 +2285,9 @@
       <c r="F21" t="s">
         <v>66</v>
       </c>
+      <c r="G21" t="s">
+        <v>264</v>
+      </c>
       <c r="H21" t="s">
         <v>94</v>
       </c>
@@ -2238,7 +2313,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>186</v>
       </c>
@@ -2255,6 +2330,9 @@
       <c r="F22" t="s">
         <v>67</v>
       </c>
+      <c r="G22" t="s">
+        <v>182</v>
+      </c>
       <c r="H22" t="s">
         <v>34</v>
       </c>
@@ -2280,7 +2358,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>186</v>
       </c>
@@ -2296,6 +2374,9 @@
       <c r="F23" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="H23" s="1" t="s">
         <v>94</v>
       </c>
@@ -2322,7 +2403,7 @@
       </c>
       <c r="S23"/>
     </row>
-    <row r="24" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>186</v>
       </c>
@@ -2338,6 +2419,9 @@
       <c r="F24" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="G24" s="9" t="s">
+        <v>175</v>
+      </c>
       <c r="H24" s="9" t="s">
         <v>53</v>
       </c>
@@ -2364,7 +2448,7 @@
       </c>
       <c r="S24"/>
     </row>
-    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>186</v>
       </c>
@@ -2381,6 +2465,9 @@
       <c r="F25" t="s">
         <v>1</v>
       </c>
+      <c r="G25" t="s">
+        <v>215</v>
+      </c>
       <c r="H25" t="s">
         <v>53</v>
       </c>
@@ -2409,7 +2496,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>186</v>
       </c>
@@ -2424,6 +2511,9 @@
       </c>
       <c r="F26" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -2454,7 +2544,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>186</v>
       </c>
@@ -2471,6 +2561,9 @@
       <c r="F27" t="s">
         <v>41</v>
       </c>
+      <c r="G27" t="s">
+        <v>180</v>
+      </c>
       <c r="H27" t="s">
         <v>47</v>
       </c>
@@ -2499,7 +2592,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>186</v>
       </c>
@@ -2516,6 +2609,9 @@
       <c r="F28" t="s">
         <v>42</v>
       </c>
+      <c r="G28" t="s">
+        <v>264</v>
+      </c>
       <c r="H28" t="s">
         <v>48</v>
       </c>
@@ -2544,7 +2640,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>186</v>
       </c>
@@ -2560,6 +2656,9 @@
       <c r="F29" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="G29" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="H29" s="1" t="s">
         <v>48</v>
       </c>
@@ -2589,7 +2688,7 @@
       </c>
       <c r="S29"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>186</v>
       </c>
@@ -2606,6 +2705,9 @@
       <c r="F30" t="s">
         <v>100</v>
       </c>
+      <c r="G30" t="s">
+        <v>178</v>
+      </c>
       <c r="H30" t="s">
         <v>33</v>
       </c>
@@ -2631,7 +2733,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>186</v>
       </c>
@@ -2648,6 +2750,9 @@
       <c r="F31" t="s">
         <v>101</v>
       </c>
+      <c r="G31" t="s">
+        <v>180</v>
+      </c>
       <c r="H31" t="s">
         <v>111</v>
       </c>
@@ -2673,7 +2778,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>186</v>
       </c>
@@ -2689,6 +2794,9 @@
       <c r="F32" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="G32" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="H32" s="1" t="s">
         <v>94</v>
       </c>
@@ -2714,7 +2822,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -2731,6 +2839,9 @@
       <c r="F33" t="s">
         <v>113</v>
       </c>
+      <c r="G33" t="s">
+        <v>264</v>
+      </c>
       <c r="H33" t="s">
         <v>48</v>
       </c>
@@ -2759,7 +2870,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>186</v>
       </c>
@@ -2776,6 +2887,9 @@
       <c r="F34" t="s">
         <v>114</v>
       </c>
+      <c r="G34" t="s">
+        <v>182</v>
+      </c>
       <c r="H34" t="s">
         <v>34</v>
       </c>
@@ -2801,7 +2915,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>186</v>
       </c>
@@ -2817,6 +2931,9 @@
       <c r="F35" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="G35" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="H35" s="1" t="s">
         <v>34</v>
       </c>
@@ -2842,7 +2959,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>186</v>
       </c>
@@ -2859,6 +2976,9 @@
       <c r="F36" t="s">
         <v>124</v>
       </c>
+      <c r="G36" t="s">
+        <v>177</v>
+      </c>
       <c r="H36" t="s">
         <v>32</v>
       </c>
@@ -2884,7 +3004,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>186</v>
       </c>
@@ -2900,6 +3020,9 @@
       <c r="F37" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="G37" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="H37" s="1" t="s">
         <v>33</v>
       </c>
@@ -2925,7 +3048,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>186</v>
       </c>
@@ -2942,6 +3065,9 @@
       <c r="F38" t="s">
         <v>130</v>
       </c>
+      <c r="G38" t="s">
+        <v>184</v>
+      </c>
       <c r="H38" t="s">
         <v>33</v>
       </c>
@@ -2970,7 +3096,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -2987,6 +3113,9 @@
       <c r="F39" t="s">
         <v>131</v>
       </c>
+      <c r="G39" t="s">
+        <v>182</v>
+      </c>
       <c r="H39" t="s">
         <v>34</v>
       </c>
@@ -3015,7 +3144,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>186</v>
       </c>
@@ -3032,6 +3161,9 @@
       <c r="F40" t="s">
         <v>132</v>
       </c>
+      <c r="G40" t="s">
+        <v>182</v>
+      </c>
       <c r="H40" t="s">
         <v>34</v>
       </c>
@@ -3060,7 +3192,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -3077,6 +3209,9 @@
       <c r="F41" t="s">
         <v>133</v>
       </c>
+      <c r="G41" t="s">
+        <v>182</v>
+      </c>
       <c r="H41" t="s">
         <v>34</v>
       </c>
@@ -3105,7 +3240,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>186</v>
       </c>
@@ -3122,6 +3257,9 @@
       <c r="F42" t="s">
         <v>134</v>
       </c>
+      <c r="G42" t="s">
+        <v>182</v>
+      </c>
       <c r="H42" t="s">
         <v>34</v>
       </c>
@@ -3147,7 +3285,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>186</v>
       </c>
@@ -3163,6 +3301,9 @@
       <c r="F43" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="G43" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="H43" s="1" t="s">
         <v>34</v>
       </c>
@@ -3191,7 +3332,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>186</v>
       </c>
@@ -3208,6 +3349,9 @@
       <c r="F44" t="s">
         <v>150</v>
       </c>
+      <c r="G44" t="s">
+        <v>264</v>
+      </c>
       <c r="H44" t="s">
         <v>94</v>
       </c>
@@ -3233,7 +3377,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>186</v>
       </c>
@@ -3249,6 +3393,9 @@
       <c r="F45" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="G45" t="s">
+        <v>266</v>
+      </c>
       <c r="H45" s="1" t="s">
         <v>35</v>
       </c>
@@ -3274,7 +3421,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>186</v>
       </c>
@@ -3291,6 +3438,9 @@
       <c r="F46" t="s">
         <v>158</v>
       </c>
+      <c r="G46" t="s">
+        <v>182</v>
+      </c>
       <c r="H46" t="s">
         <v>34</v>
       </c>
@@ -3319,7 +3469,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>186</v>
       </c>
@@ -3336,6 +3486,9 @@
       <c r="F47" t="s">
         <v>159</v>
       </c>
+      <c r="G47" t="s">
+        <v>182</v>
+      </c>
       <c r="H47" t="s">
         <v>34</v>
       </c>
@@ -3361,7 +3514,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>186</v>
       </c>
@@ -3378,6 +3531,9 @@
       <c r="F48" t="s">
         <v>160</v>
       </c>
+      <c r="G48" t="s">
+        <v>266</v>
+      </c>
       <c r="H48" t="s">
         <v>35</v>
       </c>
@@ -3403,7 +3559,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>186</v>
       </c>
@@ -3419,6 +3575,9 @@
       <c r="F49" s="4" t="s">
         <v>161</v>
       </c>
+      <c r="G49" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="H49" s="4" t="s">
         <v>34</v>
       </c>
@@ -3444,49 +3603,52 @@
         <v>182</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="12" t="s">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>235</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="B50"/>
+      <c r="C50" t="s">
         <v>240</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" t="s">
         <v>236</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" t="s">
         <v>237</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" t="s">
         <v>238</v>
       </c>
-      <c r="J50" s="13">
+      <c r="G50" t="s">
+        <v>196</v>
+      </c>
+      <c r="J50" s="2">
         <v>0</v>
       </c>
-      <c r="K50" s="13" t="s">
+      <c r="K50" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="M50" s="12" t="s">
+      <c r="M50" t="s">
         <v>219</v>
       </c>
-      <c r="N50" s="14"/>
-      <c r="O50" s="12" t="s">
+      <c r="O50" t="s">
         <v>217</v>
       </c>
-      <c r="P50" s="12" t="s">
+      <c r="P50" t="s">
         <v>220</v>
       </c>
-      <c r="Q50" s="12" t="s">
+      <c r="Q50" t="s">
         <v>220</v>
       </c>
-      <c r="R50" s="15" t="s">
+      <c r="R50" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="T50" s="12" t="s">
+      <c r="T50" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>179</v>
       </c>
@@ -3528,16 +3690,16 @@
         <v>217</v>
       </c>
       <c r="P51" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="Q51" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="R51" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>179</v>
       </c>
@@ -3591,7 +3753,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>179</v>
       </c>
@@ -3642,7 +3804,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>179</v>
       </c>
@@ -3694,7 +3856,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -3745,7 +3907,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>179</v>
       </c>
@@ -3796,7 +3958,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>179</v>
       </c>
@@ -3851,7 +4013,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>179</v>
       </c>
@@ -3903,10 +4065,10 @@
         <v>182</v>
       </c>
       <c r="T58" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -3949,19 +4111,19 @@
         <v>222</v>
       </c>
       <c r="P59" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q59" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="R59" t="s">
         <v>182</v>
       </c>
       <c r="T59" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>179</v>
       </c>
@@ -4013,7 +4175,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>179</v>
       </c>
@@ -4065,7 +4227,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -4117,7 +4279,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>179</v>
       </c>
@@ -4169,7 +4331,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>179</v>
       </c>
@@ -4221,10 +4383,10 @@
         <v>200</v>
       </c>
       <c r="T64" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>179</v>
       </c>
@@ -4279,7 +4441,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>179</v>
       </c>
@@ -4331,7 +4493,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>179</v>
       </c>
@@ -4383,7 +4545,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>179</v>
       </c>
@@ -4435,1189 +4597,247 @@
         <v>184</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69"/>
       <c r="B69"/>
       <c r="J69"/>
       <c r="K69"/>
       <c r="N69"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70"/>
       <c r="J70"/>
       <c r="K70"/>
       <c r="N70"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71"/>
       <c r="J71"/>
       <c r="K71"/>
       <c r="N71"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72"/>
       <c r="J72"/>
       <c r="K72"/>
       <c r="N72"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73"/>
       <c r="B73"/>
       <c r="J73"/>
       <c r="K73"/>
       <c r="N73"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74"/>
       <c r="B74"/>
       <c r="J74"/>
       <c r="K74"/>
       <c r="N74"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75"/>
       <c r="B75"/>
       <c r="J75"/>
       <c r="K75"/>
       <c r="N75"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76"/>
       <c r="B76"/>
       <c r="J76"/>
       <c r="K76"/>
       <c r="N76"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77"/>
       <c r="B77"/>
       <c r="J77"/>
       <c r="K77"/>
       <c r="N77"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78"/>
       <c r="B78"/>
       <c r="J78"/>
       <c r="K78"/>
       <c r="N78"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79"/>
       <c r="B79"/>
       <c r="J79"/>
       <c r="K79"/>
       <c r="N79"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80"/>
       <c r="B80"/>
       <c r="J80"/>
       <c r="K80"/>
       <c r="N80"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="J81"/>
-      <c r="K81"/>
-      <c r="N81"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="J82"/>
-      <c r="K82"/>
-      <c r="N82"/>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="J83"/>
-      <c r="K83"/>
-      <c r="N83"/>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="J84"/>
-      <c r="K84"/>
-      <c r="N84"/>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="J85"/>
-      <c r="K85"/>
-      <c r="N85"/>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="J86"/>
-      <c r="K86"/>
-      <c r="N86"/>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="J87"/>
-      <c r="K87"/>
-      <c r="N87"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="J88"/>
-      <c r="K88"/>
-      <c r="N88"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="J89"/>
-      <c r="K89"/>
-      <c r="N89"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="J90"/>
-      <c r="K90"/>
-      <c r="N90"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A91"/>
-      <c r="B91"/>
-      <c r="J91"/>
-      <c r="K91"/>
-      <c r="N91"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="J92"/>
-      <c r="K92"/>
-      <c r="N92"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="J93"/>
-      <c r="K93"/>
-      <c r="N93"/>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="J94"/>
-      <c r="K94"/>
-      <c r="N94"/>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="J95"/>
-      <c r="K95"/>
-      <c r="N95"/>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A96"/>
-      <c r="B96"/>
-      <c r="J96"/>
-      <c r="K96"/>
-      <c r="N96"/>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A97"/>
-      <c r="B97"/>
-      <c r="J97"/>
-      <c r="K97"/>
-      <c r="N97"/>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A98"/>
-      <c r="B98"/>
-      <c r="J98"/>
-      <c r="K98"/>
-      <c r="N98"/>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A99"/>
-      <c r="B99"/>
-      <c r="J99"/>
-      <c r="K99"/>
-      <c r="N99"/>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="J100"/>
-      <c r="K100"/>
-      <c r="N100"/>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="J101"/>
-      <c r="K101"/>
-      <c r="N101"/>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="J102"/>
-      <c r="K102"/>
-      <c r="N102"/>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="J103"/>
-      <c r="K103"/>
-      <c r="N103"/>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="J104"/>
-      <c r="K104"/>
-      <c r="N104"/>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="J105"/>
-      <c r="K105"/>
-      <c r="N105"/>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A106"/>
-      <c r="B106"/>
-      <c r="J106"/>
-      <c r="K106"/>
-      <c r="N106"/>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A107"/>
-      <c r="B107"/>
-      <c r="J107"/>
-      <c r="K107"/>
-      <c r="N107"/>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A108"/>
-      <c r="B108"/>
-      <c r="J108"/>
-      <c r="K108"/>
-      <c r="N108"/>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A109"/>
-      <c r="B109"/>
-      <c r="J109"/>
-      <c r="K109"/>
-      <c r="N109"/>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A110"/>
-      <c r="B110"/>
-      <c r="J110"/>
-      <c r="K110"/>
-      <c r="N110"/>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A111"/>
-      <c r="B111"/>
-      <c r="J111"/>
-      <c r="K111"/>
-      <c r="N111"/>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A112"/>
-      <c r="B112"/>
-      <c r="J112"/>
-      <c r="K112"/>
-      <c r="N112"/>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A113"/>
-      <c r="B113"/>
-      <c r="J113"/>
-      <c r="K113"/>
-      <c r="N113"/>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A114"/>
-      <c r="B114"/>
-      <c r="J114"/>
-      <c r="K114"/>
-      <c r="N114"/>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A115"/>
-      <c r="B115"/>
-      <c r="J115"/>
-      <c r="K115"/>
-      <c r="N115"/>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A116"/>
-      <c r="B116"/>
-      <c r="J116"/>
-      <c r="K116"/>
-      <c r="N116"/>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A117"/>
-      <c r="B117"/>
-      <c r="J117"/>
-      <c r="K117"/>
-      <c r="N117"/>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A118"/>
-      <c r="B118"/>
-      <c r="J118"/>
-      <c r="K118"/>
-      <c r="N118"/>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A119"/>
-      <c r="B119"/>
-      <c r="J119"/>
-      <c r="K119"/>
-      <c r="N119"/>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A120"/>
-      <c r="B120"/>
-      <c r="J120"/>
-      <c r="K120"/>
-      <c r="N120"/>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A121"/>
-      <c r="B121"/>
-      <c r="J121"/>
-      <c r="K121"/>
-      <c r="N121"/>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A122"/>
-      <c r="B122"/>
-      <c r="J122"/>
-      <c r="K122"/>
-      <c r="N122"/>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A123"/>
-      <c r="B123"/>
-      <c r="J123"/>
-      <c r="K123"/>
-      <c r="N123"/>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A124"/>
-      <c r="B124"/>
-      <c r="J124"/>
-      <c r="K124"/>
-      <c r="N124"/>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A125"/>
-      <c r="B125"/>
-      <c r="J125"/>
-      <c r="K125"/>
-      <c r="N125"/>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A126"/>
-      <c r="B126"/>
-      <c r="J126"/>
-      <c r="K126"/>
-      <c r="N126"/>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A127"/>
-      <c r="B127"/>
-      <c r="J127"/>
-      <c r="K127"/>
-      <c r="N127"/>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A128"/>
-      <c r="B128"/>
-      <c r="J128"/>
-      <c r="K128"/>
-      <c r="N128"/>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A129"/>
-      <c r="B129"/>
-      <c r="J129"/>
-      <c r="K129"/>
-      <c r="N129"/>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A130"/>
-      <c r="B130"/>
-      <c r="J130"/>
-      <c r="K130"/>
-      <c r="N130"/>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A131"/>
-      <c r="B131"/>
-      <c r="J131"/>
-      <c r="K131"/>
-      <c r="N131"/>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A132"/>
-      <c r="B132"/>
-      <c r="J132"/>
-      <c r="K132"/>
-      <c r="N132"/>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A133"/>
-      <c r="B133"/>
-      <c r="J133"/>
-      <c r="K133"/>
-      <c r="N133"/>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A134"/>
-      <c r="B134"/>
-      <c r="J134"/>
-      <c r="K134"/>
-      <c r="N134"/>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A135"/>
-      <c r="B135"/>
-      <c r="J135"/>
-      <c r="K135"/>
-      <c r="N135"/>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A136"/>
-      <c r="B136"/>
-      <c r="J136"/>
-      <c r="K136"/>
-      <c r="N136"/>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A137"/>
-      <c r="B137"/>
-      <c r="J137"/>
-      <c r="K137"/>
-      <c r="N137"/>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A138"/>
-      <c r="B138"/>
-      <c r="J138"/>
-      <c r="K138"/>
-      <c r="N138"/>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A139"/>
-      <c r="B139"/>
-      <c r="J139"/>
-      <c r="K139"/>
-      <c r="N139"/>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A140"/>
-      <c r="B140"/>
-      <c r="J140"/>
-      <c r="K140"/>
-      <c r="N140"/>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A141"/>
-      <c r="B141"/>
-      <c r="J141"/>
-      <c r="K141"/>
-      <c r="N141"/>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A142"/>
-      <c r="B142"/>
-      <c r="J142"/>
-      <c r="K142"/>
-      <c r="N142"/>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A143"/>
-      <c r="B143"/>
-      <c r="J143"/>
-      <c r="K143"/>
-      <c r="N143"/>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A144"/>
-      <c r="B144"/>
-      <c r="J144"/>
-      <c r="K144"/>
-      <c r="N144"/>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A145"/>
-      <c r="B145"/>
-      <c r="J145"/>
-      <c r="K145"/>
-      <c r="N145"/>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A146"/>
-      <c r="B146"/>
-      <c r="J146"/>
-      <c r="K146"/>
-      <c r="N146"/>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A147"/>
-      <c r="B147"/>
-      <c r="J147"/>
-      <c r="K147"/>
-      <c r="N147"/>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A148"/>
-      <c r="B148"/>
-      <c r="J148"/>
-      <c r="K148"/>
-      <c r="N148"/>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A149"/>
-      <c r="B149"/>
-      <c r="J149"/>
-      <c r="K149"/>
-      <c r="N149"/>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A150"/>
-      <c r="B150"/>
-      <c r="J150"/>
-      <c r="K150"/>
-      <c r="N150"/>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A151"/>
-      <c r="B151"/>
-      <c r="J151"/>
-      <c r="K151"/>
-      <c r="N151"/>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A152"/>
-      <c r="B152"/>
-      <c r="J152"/>
-      <c r="K152"/>
-      <c r="N152"/>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A153"/>
-      <c r="B153"/>
-      <c r="J153"/>
-      <c r="K153"/>
-      <c r="N153"/>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A154"/>
-      <c r="B154"/>
-      <c r="J154"/>
-      <c r="K154"/>
-      <c r="N154"/>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A155"/>
-      <c r="B155"/>
-      <c r="J155"/>
-      <c r="K155"/>
-      <c r="N155"/>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A156"/>
-      <c r="B156"/>
-      <c r="J156"/>
-      <c r="K156"/>
-      <c r="N156"/>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A157"/>
-      <c r="B157"/>
-      <c r="J157"/>
-      <c r="K157"/>
-      <c r="N157"/>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A158"/>
-      <c r="B158"/>
-      <c r="J158"/>
-      <c r="K158"/>
-      <c r="N158"/>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A159"/>
-      <c r="B159"/>
-      <c r="J159"/>
-      <c r="K159"/>
-      <c r="N159"/>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A160"/>
-      <c r="B160"/>
-      <c r="J160"/>
-      <c r="K160"/>
-      <c r="N160"/>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A161"/>
-      <c r="B161"/>
-      <c r="J161"/>
-      <c r="K161"/>
-      <c r="N161"/>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A162"/>
-      <c r="B162"/>
-      <c r="J162"/>
-      <c r="K162"/>
-      <c r="N162"/>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A163"/>
-      <c r="B163"/>
-      <c r="J163"/>
-      <c r="K163"/>
-      <c r="N163"/>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A164"/>
-      <c r="B164"/>
-      <c r="J164"/>
-      <c r="K164"/>
-      <c r="N164"/>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A165"/>
-      <c r="B165"/>
-      <c r="J165"/>
-      <c r="K165"/>
-      <c r="N165"/>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A166"/>
-      <c r="B166"/>
-      <c r="J166"/>
-      <c r="K166"/>
-      <c r="N166"/>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A167"/>
-      <c r="B167"/>
-      <c r="J167"/>
-      <c r="K167"/>
-      <c r="N167"/>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A168"/>
-      <c r="B168"/>
-      <c r="J168"/>
-      <c r="K168"/>
-      <c r="N168"/>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A169"/>
-      <c r="B169"/>
-      <c r="J169"/>
-      <c r="K169"/>
-      <c r="N169"/>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A170"/>
-      <c r="B170"/>
-      <c r="J170"/>
-      <c r="K170"/>
-      <c r="N170"/>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A171"/>
-      <c r="B171"/>
-      <c r="J171"/>
-      <c r="K171"/>
-      <c r="N171"/>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A172"/>
-      <c r="B172"/>
-      <c r="J172"/>
-      <c r="K172"/>
-      <c r="N172"/>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A173"/>
-      <c r="B173"/>
-      <c r="J173"/>
-      <c r="K173"/>
-      <c r="N173"/>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A174"/>
-      <c r="B174"/>
-      <c r="J174"/>
-      <c r="K174"/>
-      <c r="N174"/>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A175"/>
-      <c r="B175"/>
-      <c r="J175"/>
-      <c r="K175"/>
-      <c r="N175"/>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A176"/>
-      <c r="B176"/>
-      <c r="J176"/>
-      <c r="K176"/>
-      <c r="N176"/>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A177"/>
-      <c r="B177"/>
-      <c r="J177"/>
-      <c r="K177"/>
-      <c r="N177"/>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A178"/>
-      <c r="B178"/>
-      <c r="J178"/>
-      <c r="K178"/>
-      <c r="N178"/>
-    </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A179"/>
-      <c r="B179"/>
-      <c r="J179"/>
-      <c r="K179"/>
-      <c r="N179"/>
-    </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A180"/>
-      <c r="B180"/>
-      <c r="J180"/>
-      <c r="K180"/>
-      <c r="N180"/>
-    </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A181"/>
-      <c r="B181"/>
-      <c r="J181"/>
-      <c r="K181"/>
-      <c r="N181"/>
-    </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A182"/>
-      <c r="B182"/>
-      <c r="J182"/>
-      <c r="K182"/>
-      <c r="N182"/>
-    </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A183"/>
-      <c r="B183"/>
-      <c r="J183"/>
-      <c r="K183"/>
-      <c r="N183"/>
-    </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A184"/>
-      <c r="B184"/>
-      <c r="J184"/>
-      <c r="K184"/>
-      <c r="N184"/>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A185"/>
-      <c r="B185"/>
-      <c r="J185"/>
-      <c r="K185"/>
-      <c r="N185"/>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A186"/>
-      <c r="B186"/>
-      <c r="J186"/>
-      <c r="K186"/>
-      <c r="N186"/>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A187"/>
-      <c r="B187"/>
-      <c r="J187"/>
-      <c r="K187"/>
-      <c r="N187"/>
-    </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A188"/>
-      <c r="B188"/>
-      <c r="J188"/>
-      <c r="K188"/>
-      <c r="N188"/>
-    </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A189"/>
-      <c r="B189"/>
-      <c r="J189"/>
-      <c r="K189"/>
-      <c r="N189"/>
-    </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A190"/>
-      <c r="B190"/>
-      <c r="J190"/>
-      <c r="K190"/>
-      <c r="N190"/>
-    </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A191"/>
-      <c r="B191"/>
-      <c r="J191"/>
-      <c r="K191"/>
-      <c r="N191"/>
-    </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A192"/>
-      <c r="B192"/>
-      <c r="J192"/>
-      <c r="K192"/>
-      <c r="N192"/>
-    </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A193"/>
-      <c r="B193"/>
-      <c r="J193"/>
-      <c r="K193"/>
-      <c r="N193"/>
-    </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A194"/>
-      <c r="B194"/>
-      <c r="J194"/>
-      <c r="K194"/>
-      <c r="N194"/>
-    </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A195"/>
-      <c r="B195"/>
-      <c r="J195"/>
-      <c r="K195"/>
-      <c r="N195"/>
-    </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A196"/>
-      <c r="B196"/>
-      <c r="J196"/>
-      <c r="K196"/>
-      <c r="N196"/>
-    </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A197"/>
-      <c r="B197"/>
-      <c r="J197"/>
-      <c r="K197"/>
-      <c r="N197"/>
-    </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A198"/>
-      <c r="B198"/>
-      <c r="J198"/>
-      <c r="K198"/>
-      <c r="N198"/>
-    </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A199"/>
-      <c r="B199"/>
-      <c r="J199"/>
-      <c r="K199"/>
-      <c r="N199"/>
-    </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A200"/>
-      <c r="B200"/>
-      <c r="J200"/>
-      <c r="K200"/>
-      <c r="N200"/>
-    </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A201"/>
-      <c r="B201"/>
-      <c r="J201"/>
-      <c r="K201"/>
-      <c r="N201"/>
-    </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A202"/>
-      <c r="B202"/>
-      <c r="J202"/>
-      <c r="K202"/>
-      <c r="N202"/>
-    </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A203"/>
-      <c r="B203"/>
-      <c r="J203"/>
-      <c r="K203"/>
-      <c r="N203"/>
-    </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A204"/>
-      <c r="B204"/>
-      <c r="J204"/>
-      <c r="K204"/>
-      <c r="N204"/>
-    </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A205"/>
-      <c r="B205"/>
-      <c r="J205"/>
-      <c r="K205"/>
-      <c r="N205"/>
-    </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A206"/>
-      <c r="B206"/>
-      <c r="J206"/>
-      <c r="K206"/>
-      <c r="N206"/>
-    </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A207"/>
-      <c r="B207"/>
-      <c r="J207"/>
-      <c r="K207"/>
-      <c r="N207"/>
-    </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A208"/>
-      <c r="B208"/>
-      <c r="J208"/>
-      <c r="K208"/>
-      <c r="N208"/>
-    </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A209"/>
-      <c r="B209"/>
-      <c r="J209"/>
-      <c r="K209"/>
-      <c r="N209"/>
-    </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A210"/>
-      <c r="B210"/>
-      <c r="J210"/>
-      <c r="K210"/>
-      <c r="N210"/>
-    </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A211"/>
-      <c r="B211"/>
-      <c r="J211"/>
-      <c r="K211"/>
-      <c r="N211"/>
-    </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A212"/>
-      <c r="B212"/>
-      <c r="J212"/>
-      <c r="K212"/>
-      <c r="N212"/>
-    </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A213"/>
-      <c r="B213"/>
-      <c r="J213"/>
-      <c r="K213"/>
-      <c r="N213"/>
-    </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A214"/>
-      <c r="B214"/>
-      <c r="J214"/>
-      <c r="K214"/>
-      <c r="N214"/>
-    </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A215"/>
-      <c r="B215"/>
-      <c r="J215"/>
-      <c r="K215"/>
-      <c r="N215"/>
-    </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A216"/>
-      <c r="B216"/>
-      <c r="J216"/>
-      <c r="K216"/>
-      <c r="N216"/>
-    </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A217"/>
-      <c r="B217"/>
-      <c r="J217"/>
-      <c r="K217"/>
-      <c r="N217"/>
-    </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A218"/>
-      <c r="B218"/>
-      <c r="J218"/>
-      <c r="K218"/>
-      <c r="N218"/>
-    </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A219"/>
-      <c r="B219"/>
-      <c r="J219"/>
-      <c r="K219"/>
-      <c r="N219"/>
-    </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A220"/>
-      <c r="B220"/>
-      <c r="J220"/>
-      <c r="K220"/>
-      <c r="N220"/>
-    </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A221"/>
-      <c r="B221"/>
-      <c r="J221"/>
-      <c r="K221"/>
-      <c r="N221"/>
-    </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A222"/>
-      <c r="B222"/>
-      <c r="J222"/>
-      <c r="K222"/>
-      <c r="N222"/>
-    </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A223"/>
-      <c r="B223"/>
-      <c r="J223"/>
-      <c r="K223"/>
-      <c r="N223"/>
-    </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A224"/>
-      <c r="B224"/>
-      <c r="J224"/>
-      <c r="K224"/>
-      <c r="N224"/>
-    </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A225"/>
-      <c r="B225"/>
-      <c r="J225"/>
-      <c r="K225"/>
-      <c r="N225"/>
-    </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A226"/>
-      <c r="B226"/>
-      <c r="J226"/>
-      <c r="K226"/>
-      <c r="N226"/>
-    </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A227"/>
-      <c r="B227"/>
-      <c r="J227"/>
-      <c r="K227"/>
-      <c r="N227"/>
-    </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A228"/>
-      <c r="B228"/>
-      <c r="J228"/>
-      <c r="K228"/>
-      <c r="N228"/>
-    </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A229"/>
-      <c r="B229"/>
-      <c r="J229"/>
-      <c r="K229"/>
-      <c r="N229"/>
-    </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A230"/>
-      <c r="B230"/>
-      <c r="J230"/>
-      <c r="K230"/>
-      <c r="N230"/>
-    </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A231"/>
-      <c r="B231"/>
-      <c r="J231"/>
-      <c r="K231"/>
-      <c r="N231"/>
-    </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A232"/>
-      <c r="B232"/>
-      <c r="J232"/>
-      <c r="K232"/>
-      <c r="N232"/>
-    </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A233"/>
-      <c r="B233"/>
-      <c r="J233"/>
-      <c r="K233"/>
-      <c r="N233"/>
-    </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A234"/>
-      <c r="B234"/>
-      <c r="J234"/>
-      <c r="K234"/>
-      <c r="N234"/>
-    </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A235"/>
-      <c r="B235"/>
-      <c r="J235"/>
-      <c r="K235"/>
-      <c r="N235"/>
-    </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A236"/>
-      <c r="B236"/>
-      <c r="J236"/>
-      <c r="K236"/>
-      <c r="N236"/>
-    </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A237"/>
-      <c r="B237"/>
-      <c r="J237"/>
-      <c r="K237"/>
-      <c r="N237"/>
-    </row>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="166" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="167" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="168" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="172" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="174" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="176" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="177" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="178" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="179" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="180" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="181" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="182" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="185" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="186" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="187" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="188" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="189" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="190" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="191" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="192" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="193" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="194" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="195" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="196" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="197" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="198" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="199" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="200" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="201" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="202" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="203" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="204" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="205" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="206" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="207" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="208" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="209" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="210" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="211" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="212" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="213" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="214" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="215" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="216" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="217" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="218" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="219" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="220" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="221" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="222" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="223" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="224" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="225" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="226" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="227" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="228" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="229" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="230" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="231" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="232" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="233" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="234" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="235" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="236" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="237" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:T68" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>